<commit_message>
feat: pass all siam xlsx
</commit_message>
<xml_diff>
--- a/src/ggsheet/patim.xlsx
+++ b/src/ggsheet/patim.xlsx
@@ -133,7 +133,7 @@
   </si>
   <si>
     <t>ฉันทาหะระณะปาริสุทธิอาหะระณานิ ปะนะ อิมิสสัง สีมายัง หัตถะปาสัง วิชะหิต๎วา นิสินนานัง ภิกขูนัง อะภาวะโต นัตถิ.
-อุตุกขานัง นามะ เอตตะกัง อะติกกันตัง, เอตตะกัง อะวะสิฏฐันติ เอวัง อุตุอาจิกขะนัง; อุตูนีธะ ปะนะ สาสะเน เหมันตะคิมหะวัสสานานัง วะเสนะ ตีณิ โหนติ. อะยัง คิมโหตุ, อัส๎มิญจะ อุตุมหิ อธิกะมาสะวะเสนะ ทะสะ อุโปสะถา , อิมินา ปักเขนะ เอโก อุโปสะโถ สัมปัตโต อัฏฐะ อุโปสะถา อะติกกันตา เอโก อุโปสะโถ อะวะสิฏโฐ, อิติ เอวัง สัพเพหิ อายัส๎มันเตหิ อุตุกขานัง ธาเรตัพพัง.
+อุตุกขานัง นามะ เอตตะกัง อะติกกันตัง, เอตตะกัง อะวะสิฏฐันติ เอวัง อุตุอาจิกขะนัง; อุตูนีธะ ปะนะ สาสะเน เหมันตะคิมหะวัสสานานัง วะเสนะ ตีณิ โหนติ. อะยัง คิมโหตุ, อัส๎มิญจะ อุตุม๎หิ อธิกะมาสะวะเสนะ ทะสะ อุโปสะถา , อิมินา ปักเขนะ เอโก อุโปสะโถ สัมปัตโต อัฏฐะ อุโปสะถา อะติกกันตา เอโก อุโปสะโถ อะวะสิฏโฐ, อิติ เอวัง สัพเพหิ อายัส๎มันเตหิ อุตุกขานัง ธาเรตัพพัง.
 (รับว่า เอวัง ภันเต พร้อมกัน)</t>
   </si>
   <si>
@@ -752,7 +752,7 @@
     <t>สญฺญาจิกาย ปน ภิกฺขุนา กุฏึ การยมาเนน อสฺสามิกํ อตฺตุทฺเทสํ ปมาณิกา กาเรตพฺพา; ตตฺริทํ ปมาณํ; ทีฆโส ทฺวาทส วิทตฺถิโย สุคตวิทตฺถิยา, ติริยํ สตฺตนฺตรา. ภิกฺขู อภิเนตพฺพา วตฺถุเทสนาย; เตหิ ภิกฺขูหิ วตฺถุํ เทเสตพฺพํ อนารมฺภํ สปริกฺกมนํ. สารมฺเภ เจ ภิกฺขุ วตฺถุสฺมึ อปริกฺกมเน สญฺญาจิกาย กุฏึ กาเรยฺย, ภิกฺขู วา อนภิเนยฺย วตฺถุเทสนาย, ปมาณํ วา อติกฺกาเมยฺย, สงฺฆาทิเสโส.</t>
   </si>
   <si>
-    <t>สัญญาจิกายะ ปะนะ ภิกขุนา กุฏิง การะยะมาเนนะ อัสสามิกัง อัตตุทเทสัง ปะมาณิกา กาเรตัพพา, ตัต๎ริทัง ปะมาณัง. ทีฆะโส ทะวาทะสะ วิทัตถิโย สุคะตะวิทัตถิยา, ติริยัง สัตตันตะรา. ภิกขู อะภิเนตัพพา วัตถุเทสะนายะ, เตหิ ภิกขูหิ วัตถุง เทเสตัพพัง อะนารัมภัง สะปะริกกะมะนัง. สารัมเภ เจ ภิกขุ วัตถุส๎มิง อะปะริกกะมะเน สัญญาจิกายะ กุฏิง กาเรยยะ, ภิกขู วา อะนะภิเนยยะ วัตถุเทสะนายะ, ปะมาณัง วา อะติกกาเมยยะ, สังฆาทิเสโส.</t>
+    <t>สัญญาจิกายะ ปะนะ ภิกขุนา กุฏิง การะยะมาเนนะ อัสสามิกัง อัตตุทเทสัง ปะมาณิกา กาเรตัพพา, ตัต๎ริทัง ปะมาณัง. ทีฆะโส ท๎วาทะสะ วิทัตถิโย สุคะตะวิทัตถิยา, ติริยัง สัตตันตะรา. ภิกขู อะภิเนตัพพา วัตถุเทสะนายะ, เตหิ ภิกขูหิ วัตถุง เทเสตัพพัง อะนารัมภัง สะปะริกกะมะนัง. สารัมเภ เจ ภิกขุ วัตถุส๎มิง อะปะริกกะมะเน สัญญาจิกายะ กุฏิง กาเรยยะ, ภิกขู วา อะนะภิเนยยะ วัตถุเทสะนายะ, ปะมาณัง วา อะติกกาเมยยะ, สังฆาทิเสโส.</t>
   </si>
   <si>
     <t>Saññācikāya pana bhikkhunā kuṭiṁ kārayamānena assāmikaṁ attuddesaṁ pamāṇikā kāretabbā, tatr’ idaṁ pamānaṁ. Dīghaso dvādasa vidatthiyo sugatavidatthiyā tiriyaṁ satt’ antarā. Bhikkhū abhinetabbā vatthudesanāya, tehi bhikkhūhi vatthuṁ desetabbaṁ anārambhaṁ saparikkamanaṁ. Sārambhe ce bhikkhu vatthusmiṁ aparikkamane saññācikāya kuṭiṁ kāreyya, bhikkhū vā anabhineyya vatthudesanāya, pamāṇaṁ vā atikkāmeyya, saṅghādiseso.</t>
@@ -776,7 +776,7 @@
     <t>โย ปน ภิกฺขุ ภิกฺขุํ ทุฏฺโฐ โทโส อปฺปตีโต อมูลเกน ปาราชิเกน ธมฺเมน อนุทฺธํเสยฺย “อปฺเปว นาม นํ อิมมฺหา พฺรหฺมจริยา จาเวยฺยนฺติ. ตโต อปเรน สมเยน สมนุคฺคาหิยมาโน วา อสมนุคฺคาหิยมาโน วา, อมูลกญฺเจว ตํ อธิกรณํ โหติ, ภิกฺขุ จ โทสํ ปติฏฺฐาติ, สงฺฆาทิเสโส.</t>
   </si>
   <si>
-    <t>โย ปะนะ ภิกขุ ภิกขุง ทุฏโฐ โทโส อัปปะตีโต อะมูละเกนะ ปาราชิเกนะ ธัมเมนะ อะนุทธังเสยยะ “อัปเปวะ นามะ นัง อิมัมหา พ๎รัห๎มะจะริยา จาเวยยันติ. ตะโต อะปะเรนะ สะมะเยนะ สะมะนุคคาหิยะมาโน วา, อะสะมะนุคคาหิยะมาโน วา, อะมูละกัญเจวะ ตัง อะธิกะระณัง โหติ, ภิกขุ จะ โทสัง ปะติฏฐาติ, สังฆาทิเสโส.</t>
+    <t>โย ปะนะ ภิกขุ ภิกขุง ทุฏโฐ โทโส อัปปะตีโต อะมูละเกนะ ปาราชิเกนะ ธัมเมนะ อะนุทธังเสยยะ “อัปเปวะ นามะ นัง อิมัม๎หา พ๎รัห๎มะจะริยา จาเวยยันติ. ตะโต อะปะเรนะ สะมะเยนะ สะมะนุคคาหิยะมาโน วา, อะสะมะนุคคาหิยะมาโน วา, อะมูละกัญเจวะ ตัง อะธิกะระณัง โหติ, ภิกขุ จะ โทสัง ปะติฏฐาติ, สังฆาทิเสโส.</t>
   </si>
   <si>
     <t>Yo pana bhikkhu bhikkhuṁ duṭṭho doso appatīto amūlakena pārājikena dhammena anuddhaṁseyya, “app’eva nāma naṁ imamhā brahmacariyā cāveyyan” ti, tato aparena samayena samanuggāhiyamāno vā asamanuggāhiyamāno vā, amūlakañ c’eva taṁ adhikaraṇaṁ hoti, bhikkhu ca dosaṁ patiṭṭhā’ ti, saṅghādiseso.</t>
@@ -788,7 +788,7 @@
     <t>โย ปน ภิกฺขุ ภิกฺขุํ ทุฏฺโฐ โทโส อปฺปตีโต อญฺญภาคิยสฺส อธิกรณสฺส กิญฺจิ เทสํ เลสมตฺตํ อุปาทาย ปาราชิเกน ธมฺเมน อนุทฺธํเสยฺย “อปฺเปว นาม นํ อิมมฺหา พฺรหฺมจริยา จาเวยฺยนฺติ, ตโต อปเรน สมเยน สมนุคฺคาหิยมาโน วา อสมนุคฺคาหิยมาโน วา, อญฺญภาคิยญฺเจว ตํ อธิกรณํ โหติ, โกจิ เทโส เลสมตฺโต อุปาทินฺโน ภิกฺขุ จ โทสํ ปติฏฺฐาติ, สงฺฆาทิเสโส.</t>
   </si>
   <si>
-    <t>โย ปะนะ ภิกขุ ภิกขุง ทุฏโฐ โทโส อัปปะตีโต อัญญะภาคิยัสสะ อะธิกะระณัสสะ กิญจิ เทสัง เลสะมัตตัง อุปาทายะ ปาราชิเกนะ ธัมเมนะ อะนุทธังเสยยะ "อัปเปวะ นามะ นัง อิมัมหา พ๎รัห๎มะจะริยา จาเวยยันติ. ตะโต อะปะเรนะ สะมะเยนะ สะมะนุคคาหิยะมาโน วา, อะสะมะนุคคาหิยะมาโน วา, อัญญะภาคิยัญเจวะ ตัง อะธิกะระณัง โหติ, โกจิ เทโส เลสะมัตโต อุปาทินโน ภิกขุ จะ โทสัง ปะติฏฐาติ, สังฆาทิเสโส.</t>
+    <t>โย ปะนะ ภิกขุ ภิกขุง ทุฏโฐ โทโส อัปปะตีโต อัญญะภาคิยัสสะ อะธิกะระณัสสะ กิญจิ เทสัง เลสะมัตตัง อุปาทายะ ปาราชิเกนะ ธัมเมนะ อะนุทธังเสยยะ "อัปเปวะ นามะ นัง อิมัม๎หา พ๎รัห๎มะจะริยา จาเวยยันติ. ตะโต อะปะเรนะ สะมะเยนะ สะมะนุคคาหิยะมาโน วา, อะสะมะนุคคาหิยะมาโน วา, อัญญะภาคิยัญเจวะ ตัง อะธิกะระณัง โหติ, โกจิ เทโส เลสะมัตโต อุปาทินโน ภิกขุ จะ โทสัง ปะติฏฐาติ, สังฆาทิเสโส.</t>
   </si>
   <si>
     <t>Yo pana bhikkhu bhikkhuṁ duṭṭho doso appatīto aññabhāgiyassa adhikaraṇassa kiñci desaṁ lesamattaṁ upādāya pārājikena dhammena anuddhaṁseyya, “app’eva nāma naṁ imamhā brahmacariyā cāveyyan” ti, tato aparena samayena samanuggāhiyamāno vā asamanuggāhiyamāno vā, aññabhāgiyañ c’eva taṁ adhikaraṇaṁ hoti, koci deso lesamatto upādinno bhikkhu ca dosaṁ patiṭṭhā’ti, saṅghādiseso.</t>
@@ -800,7 +800,7 @@
     <t>โย ปน ภิกฺขุ สมคฺคสฺส สงฺฆสฺส เภทาย ปรกฺกเมยฺย เภทนสํวตฺตนิกํ วา อธิกรณํ สมาทาย ปคฺคยฺห ติฏฺเฐยฺย. โส ภิกฺขุ ภิกฺขูหิ เอวมสฺส วจนีโย “มา อายสฺมา สมคฺคสฺส สงฺฆสฺส เภทาย ปรกฺกมิ, เภทนสํวตฺตนิกํ วา อธิกรณํ สมาทาย ปคฺคยฺห อฏฺฐาสิ; สเมตายสฺมา สงฺเฆน, สมคฺโค หิ สงฺโฆ สมฺโมทมาโน อวิวทมาโน เอกุทฺเทโส ผาสุ วิหรตีติ. เอวญฺจ โส ภิกฺขุ ภิกฺขูหิ วุจฺจมาโน ตเถว ปคฺคณฺเหยฺย, โส ภิกฺขุ ภิกฺขูหิ ยาวตติยํ สมนุภาสิตพฺโพ ตสฺส ปฏินิสฺสคฺคาย; ยาวตติยญฺเจ สมนุภาสิยมาโน ตํ ปฏินิสฺสชฺเชยฺย, อิจฺเจตํ กุสลํ; โน เจ ปฏินิสฺสชฺเชยฺย, สงฺฆาทิเสโส.</t>
   </si>
   <si>
-    <t>โย ปะนะ ภิกขุ สะมัคคัสสะ สังฆัสสะ เภทายะ ปะรักกะเมยยะ เภทะนะสังวัตตะนิกัง วา อะธิกะระณัง สะมาทายะ ปัคคัยหะ ติฏเฐยยะ. โส ภิกขุ ภิกขูหิ เอวะมัสสะ วะจะนีโย "มา อายัส๎มา สะมัคคัสสะ สังฆัสสะ เภทายะ ปะรักกะมิ, เภทะนะสังวัตตะนิกัง วา อะธิกะระณัง สะมาทายะ ปัคคัยหะ อัฏฐาสิ, สะเมตายัส๎มา สังเฆนะ, สะมัคโค หิ สังโฆ สัมโมทะมาโน อะวิวะทะมาโน เอกุทเทโส ผาสุ วิหะระตีติ. เอวัญจะ โส ภิกขุ ภิกขูหิ วุจจะมาโน ตะเถวะ ปัคคัณเหยยะ, โส ภิกขุ ภิกขูหิ ยาวะตะติยัง สะมะนุภาสิตัพโพ ตัสสะ ปะฏินิสสัคคายะ, ยาวะ ตะติยัญเจ สะมะนุภาสิยะมาโน ตัง ปะฏินิสสัชเชยยะ, อิจเจตัง กุสะลัง, โน เจ ปะฏินิสสัชเชยยะ , สังฆาทิเสโส.</t>
+    <t>โย ปะนะ ภิกขุ สะมัคคัสสะ สังฆัสสะ เภทายะ ปะรักกะเมยยะ เภทะนะสังวัตตะนิกัง วา อะธิกะระณัง สะมาทายะ ปัคคัยหะ ติฏเฐยยะ. โส ภิกขุ ภิกขูหิ เอวะมัสสะ วะจะนีโย "มา อายัส๎มา สะมัคคัสสะ สังฆัสสะ เภทายะ ปะรักกะมิ, เภทะนะสังวัตตะนิกัง วา อะธิกะระณัง สะมาทายะ ปัคคัยหะ อัฏฐาสิ, สะเมตายัส๎มา สังเฆนะ, สะมัคโค หิ สังโฆ สัมโมทะมาโน อะวิวะทะมาโน เอกุทเทโส ผาสุ วิหะระตีติ. เอวัญจะ โส ภิกขุ ภิกขูหิ วุจจะมาโน ตะเถวะ ปัคคัณเหยยะ, โส ภิกขุ ภิกขูหิ ยาวะตะติยัง สะมะนุภาสิตัพโพ ตัสสะ ปะฏินิสสัคคายะ, ยาวะตะติยัญเจ สะมะนุภาสิยะมาโน ตัง ปะฏินิสสัชเชยยะ, อิจเจตัง กุสะลัง, โน เจ ปะฏินิสสัชเชยยะ , สังฆาทิเสโส.</t>
   </si>
   <si>
     <t>Yo pana bhikkhu samaggassa saṅghassa bhedāya parakkameyya bhedanasaṁvattanikaṁ vā adhikaraṇaṁ samādāya paggayha tiṭṭheyya, so bhikkhu bhikkhūhi evam assa vacanīyo “Mā āyasmā samaggassa saṅghassa bhedāya parakkami bhedanasaṁvattanikaṁ vā adhikaraṇaṁ samādāya paggayha aṭṭhāsi, samet’ āyasmā saṅghena, samaggo hi saṅgho sammodamāno avivadamāno ekuddeso phāsu viharatī”ti. Evañca so bhikkhu bhikkhūhi vuccamāno tath’eva paggaṇheyya, so bhikkhu bhikkhūhi yāvatatiyaṁ samanubhāsitabbo tassa paṭinissaggāya, yāvatatiyañ’ce samanubhāsiyamāno taṁ paṭinissajjeyya icc’etaṁ kusalaṁ. No ce paṭinissajjeyya, saṅghādiseso.</t>
@@ -812,7 +812,7 @@
     <t>ตสฺเสว โข ปน ภิกฺขุสฺส ภิกฺขู โหนฺติ อนุวตฺตกา วคฺควาทกา, เอโก วา เทฺว วา ตโย วา, เต เอวํ วเทยฺยุํ, “มา อายสฺมนฺโต เอตํ ภิกฺขุํ กิญฺจิ อวจุตฺถ ธมฺมวาที เจโส ภิกฺขุ, วินยวาที เจโส ภิกฺขุ, อมฺหากญฺเจโส ภิกฺขุ, ฉนฺทญฺจ รุจิญฺจ อาทาย โวหรติ, ชานาติ โน ภาสติ, อมฺหากมฺเปตํ ขมตีติ. เต ภิกฺขู ภิกฺขูหิ เอวมสฺสุ วจนียา “มา อายสฺมนฺโต เอวํ อวจุตฺถ, น เจโส ภิกฺขุ ธมฺมวาที, น เจโส ภิกฺขุ วินยวาที, มา อายสฺมนฺตานมฺปิ สงฺฆเภโท รุจิตฺถ, สเมตายสฺมนฺตานํ สงฺเฆน, สมคฺโค หิ สงฺโฆ สมฺโมทมาโน อวิวทมาโน เอกุทฺเทโส ผาสุ วิหรตีติ. เอวญฺจ เต ภิกฺขู ภิกฺขูหิ วุจฺจมานา ตเถว ปคฺคณฺเหยฺยุํ, เต ภิกฺขู ภิกฺขูหิ ยาวตติยํ สมนุภาสิตพฺพา ตสฺส ปฏินิสฺสคฺคาย; ยาวตติยญฺเจ สมนุภาสิยมานา ตํ ปฏินิสฺสชฺเชยฺยุํ อิจฺเจตํ กุสลํ, โน เจ ปฏินิสฺสชฺเชยฺยุํ; สงฺฆาทิเสโส.</t>
   </si>
   <si>
-    <t>ตัสเสวะ โข ปะนะ ภิกขุสสะ ภิกขู โหนติ อะนุวัตตะกา วัคคะวาทะกา, เอโก วา เท๎ว วา ตะโย วา, เต เอวัง วะเทยยุง, “มา อายัส๎มันโต เอตัง ภิกขุง กิญจิ อะวะจุตถะ ธัมมะวาที เจโส ภิกขุ, วินะยะวาที เจโส ภิกขุ, อัมหากัญเจโส ภิกขุ, ฉันทัญจะ รุจิญจะ อาทายะ โวหะระติ, ชานาติ โน ภาสะติ, อัมหากัมเปตัง ขะมะตีติ. เต ภิกขู ภิกขูหิ เอวะมัสสุ วะจะนียา “มา อายัส๎มันโต เอวัง อะวะจุตถะ, นะ เจโส ภิกขุ ธัมมะวาที, นะ เจโส ภิกขุ วินะยะวาที, มา อายัส๎มันตานัมปิ สังฆะเภโท รุจิตถะ, สะเมตายัส๎มันตานัง สังเฆนะ, สะมัคโค หิ สังโฆ สัมโมทะมาโน อะวิวะทะมาโน เอกุทเทโส ผาสุ วิหะระตีติ. เอวัญจะ เต ภิกขู ภิกขูหิ วุจจะมานา ตะเถวะ ปัคคัณเหยยุง, เต ภิกขู ภิกขูหิ ยาวะตะติยัง สะมะนุภาสิตัพพา ตัสสะ ปะฏินิสสัคคายะ, ยาวะตะติยัญเจ สะมะนุภาสิยะมานา ตัง ปะฏินิสสัชเชยยุง, อิจเจตัง กุสะลัง, โน เจ ปะฏินิสสัชเชยยุง, สังฆาทิเสโส.</t>
+    <t>ตัสเสวะ โข ปะนะ ภิกขุสสะ ภิกขู โหนติ อะนุวัตตะกา วัคคะวาทะกา, เอโก วา เท๎ว วา ตะโย วา, เต เอวัง วะเทยยุง, “มา อายัส๎มันโต เอตัง ภิกขุง กิญจิ อะวะจุตถะ ธัมมะวาที เจโส ภิกขุ, วินะยะวาที เจโส ภิกขุ, อัม๎หากัญเจโส ภิกขุ, ฉันทัญจะ รุจิญจะ อาทายะ โวหะระติ, ชานาติ โน ภาสะติ, อัม๎หากัมเปตัง ขะมะตีติ. เต ภิกขู ภิกขูหิ เอวะมัสสุ วะจะนียา “มา อายัส๎มันโต เอวัง อะวะจุตถะ, นะ เจโส ภิกขุ ธัมมะวาที, นะ เจโส ภิกขุ วินะยะวาที, มา อายัส๎มันตานัมปิ สังฆะเภโท รุจิตถะ, สะเมตายัส๎มันตานัง สังเฆนะ, สะมัคโค หิ สังโฆ สัมโมทะมาโน อะวิวะทะมาโน เอกุทเทโส ผาสุ วิหะระตีติ. เอวัญจะ เต ภิกขู ภิกขูหิ วุจจะมานา ตะเถวะ ปัคคัณเหยยุง, เต ภิกขู ภิกขูหิ ยาวะตะติยัง สะมะนุภาสิตัพพา ตัสสะ ปะฏินิสสัคคายะ, ยาวะตะติยัญเจ สะมะนุภาสิยะมานา ตัง ปะฏินิสสัชเชยยุง, อิจเจตัง กุสะลัง, โน เจ ปะฏินิสสัชเชยยุง, สังฆาทิเสโส.</t>
   </si>
   <si>
     <t>Tass’eva kho pana bhikkhussa bhikkhū honti anuvattakā vaggavādakā, eko vā dve vā tayo vā, te evaṁ vadeyyuṁ, “Mā āyasmanto etaṁ bhikhhuṁ kiñci avacuttha, dhammavādī c’eso bhikkhu, vinayavādī c’eso bhikkhu, amhākañc’eso bhikkhu, chandañca ruciñca ādāya voharati, jānāti no bhāsati, amhākamp’etaṁ khamatī”ti. Te bhikkhū bhikkhūhi evam assu vacanīyā, “Mā āyasmanto evaṁ avacuttha. Na c’eso bhikkhu dhammavādī na c’eso bhikkhu vinayavādī. Mā āyasmantānam’pi saṅghabhedo rucittha, samet’āyasmantānaṁ saṅghena, samaggo hi saṅgho sammodamāno avivadamāno. Ekuddeso phāsu viharatī”ti. Evañca te bhikkhū bhikkhūhi vuccamānā tath’eva paggaṇheyyuṁ, te bhikkhū bhikkhūhi yāvatatiyaṁ samanubhāsitabbā tassa paṭinissaggāya, yāvatatiyañce samanubhāsiyamānā taṁ paṭinissajjeyyuṁ icc’etaṁ kusalaṁ, no ce paṭinissajjeyyuṁ, sanghādiseso.</t>
@@ -836,7 +836,7 @@
     <t>ภิกฺขุ ปเนว อญฺญตรํ คามํ วา นิคมํ วา อุปนิสฺสาย วิหรติ กุลทูสโก ปาปสมาจาโร, ตสฺส โข ปาปกา สมาจารา ทิสฺสนฺติ เจว สุยฺยนฺติ จ, กุลานิ จ เตน ทุฏฺฐานิ ทิสฺสนฺติ เจว สุยฺยนฺติ จ. โส ภิกฺขุ ภิกฺขูหิ เอวมสฺส วจนีโย “อายสฺมา โข กุลทูสโก ปาปสมาจาโร, อายสฺมโต โข ปาปกา สมาจารา ทิสฺสนฺติ เจว สุยฺยนฺติ จ. กุลานิ จายสฺมตา ทุฏฺฐานิ ทิสฺสนฺติ เจว สุยฺยนฺติ จ; ปกฺกมตายสฺมา อิมมฺหา อาวาสา, อลนฺเต อิธ วาเสนาติ. เอวญฺจ โส ภิกฺขุ ภิกฺขูหิ วุจฺจมาโน เต ภิกฺขู เอวํ วเทยฺย “ฉนฺทคามิโน จ ภิกฺขู, โทสคามิโน จ ภิกฺขู, โมหคามิโน จ ภิกฺขู, ภยคามิโน จ ภิกฺขู; ตาทิสิกาย อาปตฺติยา เอกจฺจํ ปพฺพาเชนฺติ, เอกจฺจํ น ปพฺพาเชนฺตีติ. โส ภิกฺขุ ภิกฺขูหิ เอวมสฺส วจนีโย “มา อายสฺมา เอวํ อวจ, น จ ภิกฺขู ฉนฺทคามิโน, น จ ภิกฺขู โทสคามิโน, น จ ภิกฺขู โมหคามิโน, น จ ภิกฺขู ภยคามิโน; อายสฺมา โข กุลทูสโก ปาปสมาจาโร, อายสฺมโต โข ปาปกา สมาจารา ทิสฺสนฺติ เจว สุยฺยนฺติ จ, กุลานิ จายสฺมตา ทุฏฺฐานิ ทิสฺสนฺติ เจว สุยฺยนฺติ จ, ปกฺกมตายสฺมา อิมมฺหา อาวาสา, อลนฺเต อิธ วาเสนาติ. เอวญฺจ โส ภิกฺขุ ภิกฺขูหิ วุจฺจมาโน ตเถว ปคฺคณฺเหยฺย, โส ภิกฺขุ ภิกฺขูหิ ยาวตติยํ สมนุภาสิตพฺโพ ตสฺส ปฏินิสฺสคฺคาย; ยาวตติยญฺเจ สมนุภาสิยมาโน ตํ ปฏินิสฺสชฺเชยฺย, อิจฺเจตํ กุสลํ; โน เจ ปฏินิสฺสชฺเชยฺย, สงฺฆาทิเสโส.</t>
   </si>
   <si>
-    <t>ภิกขุ ปะเนวะ อัญญะตะรัง คามัง วา นิคะมัง วา อุปะนิสสายะ วิหะระติ กุละทูสะโก ปาปะสะมาจาโร, ตัสสะ โข ปาปะกา สะมาจารา ทิสสันติ เจวะ สุยยันติ จะ, กุลานิ จะ เตนะ ทุฏฐานิ ทิสสันติ เจวะ สุยยันติ จะ. โส ภิกขุ ภิกขูหิ เอวะมัสสะ วะจะนีโย "อายัส๎มา โข กุละทูสะโก ปาปะสะมาจาโร, อายัส๎มะโต โข ปาปะกา สะมาจารา ทิสสันติ เจวะ สุยยันติ จะ. กุลานิ จายัส๎มะตา ทุฏฐานิ ทิสสันติ เจวะ สุยยันติ จะ, ปักกะมะตายัส๎มา อิมัมหา อาวาสา, อะลันเต อิธะ วาเสนาติ. เอวัญจะ โส ภิกขุ ภิกขูหิ วุจจะมาโน เต ภิกขู เอวัง วะเทยยะ “ฉันทะคามิโน จะ ภิกขู, โทสะคามิโน จะ ภิกขู, โมหะคามิโน จะ ภิกขู, ภะยะคามิโน จะ ภิกขู, ตาทิสิกายะ อาปัตติยา เอกัจจัง ปัพพาเชนติ, เอกัจจัง นะ ปัพพาเชนตีติ. โส ภิกขุ ภิกขูหิ เอวะมัสสะ วะจะนีโย “มา อายัส๎มา เอวัง อะวะจะ, นะ จะ ภิกขู ฉันทะคามิโน, นะ จะ ภิกขู โทสะคามิโน, นะ จะ ภิกขู โมหะคามิโน, นะ จะ ภิกขู ภะยะคามิโน, อายัส๎มา โข กุละทูสะโก ปาปะสะมาจาโร, อายัส๎มะโต โข ปาปะกาสะมาจารา ทิสสันติ เจวะ สุยยันติ จะ, กุลานิ จายัส๎มะตา ทุฏฐานิ ทิสสันติ เจวะ สุยยันติ จะ, ปักกะมะตายัส๎มา อิมัมหา อาวาสา, อะลันเต อิธะ วาเสนาติ. เอวัญจะ โส ภิกขุ ภิกขูหิ วุจจะมาโน ตะเถวะ ปัคคัณเหยยะ, โส ภิกขุ ภิกขูหิ ยาวะตะติยัง สะมานุภาสิตัพโพ ตัสสะ ปะฏินิสสัคคายะ, ยาวะตะติยัญเจ สะมะนุภาสิยะมาโน ตัง ปะฏินิสสัชเชยยะ, อิจเจตัง กุสะลัง, โน เจ ปะฏินิสสัชเชยยะ, สังฆาทิเสโส.</t>
+    <t>ภิกขุ ปะเนวะ อัญญะตะรัง คามัง วา นิคะมัง วา อุปะนิสสายะ วิหะระติ กุละทูสะโก ปาปะสะมาจาโร, ตัสสะ โข ปาปะกา สะมาจารา ทิสสันติ เจวะ สุยยันติ จะ, กุลานิ จะ เตนะ ทุฏฐานิ ทิสสันติ เจวะ สุยยันติ จะ. โส ภิกขุ ภิกขูหิ เอวะมัสสะ วะจะนีโย "อายัส๎มา โข กุละทูสะโก ปาปะสะมาจาโร, อายัส๎มะโต โข ปาปะกา สะมาจารา ทิสสันติ เจวะ สุยยันติ จะ. กุลานิ จายัส๎มะตา ทุฏฐานิ ทิสสันติ เจวะ สุยยันติ จะ, ปักกะมะตายัส๎มา อิมัม๎หา อาวาสา, อะลันเต อิธะ วาเสนาติ. เอวัญจะ โส ภิกขุ ภิกขูหิ วุจจะมาโน เต ภิกขู เอวัง วะเทยยะ “ฉันทะคามิโน จะ ภิกขู, โทสะคามิโน จะ ภิกขู, โมหะคามิโน จะ ภิกขู, ภะยะคามิโน จะ ภิกขู, ตาทิสิกายะ อาปัตติยา เอกัจจัง ปัพพาเชนติ, เอกัจจัง นะ ปัพพาเชนตีติ. โส ภิกขุ ภิกขูหิ เอวะมัสสะ วะจะนีโย “มา อายัส๎มา เอวัง อะวะจะ, นะ จะ ภิกขู ฉันทะคามิโน, นะ จะ ภิกขู โทสะคามิโน, นะ จะ ภิกขู โมหะคามิโน, นะ จะ ภิกขู ภะยะคามิโน, อายัส๎มา โข กุละทูสะโก ปาปะสะมาจาโร, อายัส๎มะโต โข ปาปะกา สะมาจารา ทิสสันติ เจวะ สุยยันติ จะ, กุลานิ จายัส๎มะตา ทุฏฐานิ ทิสสันติ เจวะ สุยยันติ จะ, ปักกะมะตายัส๎มา อิมัม๎หา อาวาสา, อะลันเต อิธะ วาเสนาติ. เอวัญจะ โส ภิกขุ ภิกขูหิ วุจจะมาโน ตะเถวะ ปัคคัณเหยยะ, โส ภิกขุ ภิกขูหิ ยาวะตะติยัง สะมะนุภาสิตัพโพ ตัสสะ ปะฏินิสสัคคายะ, ยาวะตะติยัญเจ สะมะนุภาสิยะมาโน ตัง ปะฏินิสสัชเชยยะ, อิจเจตัง กุสะลัง, โน เจ ปะฏินิสสัชเชยยะ, สังฆาทิเสโส.</t>
   </si>
   <si>
     <t>Bhikkhu pan’eva aññataraṁ gāmaṁ vā nigamaṁ vā upanissāya viharati kuladūsako pāpasamācāro, tassa kho pāpakā samācārā dissanti c’eva suyyanti ca, kulāni ca tena duṭṭhāni dissanti c’eva suyyanti ca. So bhikkhu bhikkhūhi evam assa vacanīyo, “Āyasmā kho kuladūsako pāpasamācāro, āyasmato kho pāpakā samācārā dissanti c’eva suyyanti ca, kulāni c’ āyasmatā duṭṭthāni dissanti c’eva suyyanti ca; pakkamat’ āyasmā imamhā āvāsā, alan’te idha vāsenā” ti. Evañca so bhikkhu bhikkhūhi vuccamāno te bhikkhū evaṁ vadeyya, “chandagāmino ca bhikkhū, dosagāmino ca bhikkhū, mohagāmino ca bhikkhū, bhayagāmino ca bhikkhū; tādisikāya āpattiyā ekaccaṁ pabbājenti, ekaccaṁ na pabbājentī” ti. So bhikkhu bhikkhūhi evam’ assa vacanīyo, “mā āyasmā evaṁ avaca, na ca bhikkhū chandagāmino, na ca bhikkhū dosagāmino, na ca bhikkhū mohagāmino, na ca bhikkhū bhayagāmino; āyasmā kho kuladūsako pāpasamācāro, āyasmato kho pāpakā samācārā dissanti c’eva suyyanti ca, kulāni c’ āyasmatā duṭṭthāni dissanti c’eva suyyanti ca, pakkamat’ āyasmā imamhā āvāsā, alan’te idha vāsenā” ti. Evañca so bhikkhu bhikkhūhi vuccamāno tath’eva paggaṇheyya, so bhikkhu bhikkhūhi yāvatatiyaṁ samanubhāsitabbo tassa paṭinissaggāya; yāvatatiyañce samanubhāsiyamāno taṁ paṭinissajjeyya, icc’etaṁ kusalaṁ; no ce paṭinissajjeya, saṅghādiseso.</t>
@@ -872,7 +872,7 @@
         <rFont val="Arial"/>
         <color theme="1"/>
       </rPr>
-      <t xml:space="preserve">อุททิฏฐา โข อายัส๎มันโต เตระสะ สังฆาทิเสสา ธัมมา. นะวะ ปะฐะมาปัตติกา, จัตตาโร ยาวะตะติยะกา, เยสัง ภิกขุ อัญญะตะรัง วา อัญญะตะรัง วา อาปัชชิต๎วา ยาวะติหัง ชานัง ปะฏิจฉาเทติ, ตาวะติหัง เตนะ ภิกขุนา อะกามา ปะริวัตถัพพัง, ปะริวุตถะปะริวาเสนะ ภิกขุนา อุตตะริง ฉารัตตัง ภิกขุมานัตตายะ ปะฏิปัชชิตัพพัง, จิณณะมานัตโต ภิกขุ, ยัตถะ สิยา วีสะติคะโณ ภิกขุสังโฆ, ตัตถะ โส ภิกขุ อัพเภตัพโพ, เอเกนะปิ เจ อูโน วีสะติคะโณ ภิกขุสังโฆ ตัง ภิกขุง อัพเภยยะ, โส จะ ภิกขุ อะนัพภิโต, เต จะ ภิกขู คารัย๎หา. อะยัง ตัตถะ สามีจิ.
+      <t xml:space="preserve">อุททิฏฐา โข อายัส๎มันโต เตระสะ สังฆาทิเสสา ธัมมา. นะวะ ปะฐะมาปัตติกา, จัตตาโร ยาวะตะติยะกา, เยสัง ภิกขุ อัญญะตะรัง วา อัญญะตะรัง วา อาปัชชิต๎วา ยาวะติหัง ชานัง ปะฏิจฉาเทติ, ตาวะติหัง เตนะ ภิกขุนา อะกามา ปะริวัตถัพพัง, ปะริวุตถะปะริวาเสนะ ภิกขุนา อุตตะริง ฉารัตตัง ภิกขุมานัตตายะ ปะฏิปัชชิตัพพัง, จิณณะมานัตโต ภิกขุ, ยัตถะ สิยา วีสะติคะโณ ภิกขุสังโฆ, ตัตถะ โส ภิกขุ อัพเภตัพโพ, เอเกนะปิ เจ อูโน วีสะติคะโณ ภิกขุ สังโฆ ตัง ภิกขุง อัพเภยยะ, โส จะ ภิกขุ อะนัพภิโต, เต จะ ภิกขู คารัย๎หา. อะยัง ตัตถะ สามีจิ.
 ตัตถายัส๎มันเต ปุจฉามิ. กัจจิตถะ ปะริสุทธา ?
 ทุติยัมปิ ปุจฉามิ. กัจจิตถะ ปะริสุทธา ?
 ตะติยัมปิ ปุจฉามิ. กัจจิตถะ ปะริสุทธา ?
@@ -1217,7 +1217,7 @@
     <t>นิฏฺฐิตจีวรสฺมึ ภิกฺขุนา อุพฺภตสฺมึ กฐิเน, เอกรตฺตมฺปิ เจ ภิกฺขุ ติจีวเรน วิปฺปวเสยฺย, อญฺญตฺร ภิกฺขุ สมฺมติยา, นิสฺสคฺคิยํ ปาจิตฺติยํ.</t>
   </si>
   <si>
-    <t>นิฏฐิตะจีวะรัส๎มิง ภิกขุนา อุพภะตัส๎มิง กะฐิเน, เอกะรัตตัมปิ เจ ภิกขุ ติจีวะเรนะ วิปปะวะเสยยะ, อัญญัต๎ระ ภิกขุสัมมะติยา, นิสสัคคิยัง ปาจิตติยัง.</t>
+    <t>นิฏฐิตะจีวะรัส๎มิง ภิกขุนา อุพภะตัส๎มิง กะฐิเน, เอกะรัตตัมปิ เจ ภิกขุ ติจีวะเรนะ วิปปะวะเสยยะ, อัญญัต๎ระ ภิกขุ สัมมะติยา, นิสสัคคิยัง ปาจิตติยัง.</t>
   </si>
   <si>
     <t>๒. จีวรสำเร็จแล้ว กฐินอันภิกษุเดาะเสียแล้ว ถ้าภิกษุอยู่ปราศจากไตรจีวรแม้สิ้นราตรีหนึ่ง เว้นเสียแต่ภิกษุได้รับสมมติเป็นนิสสัคคิยปาจิตตีย์.</t>
@@ -1298,7 +1298,7 @@
     <t>ภิกฺขุํ ปเนว อุทฺทิสฺส อุภินฺนํ อญฺญาตกานํ คหปตีนํ วา คหปตานีนํ วา ปจฺเจกจีวรเจตาปนา อุปกฺขฏา โหนฺติ “อิเมหิ มยํ ปจฺเจกจีวรเจตาปเนหิ ปจฺเจกจีวรานิ เจตาเปตฺวา อิตฺถนฺนามํ ภิกฺขุํ จีวเรหิ อจฺฉาเทสฺสามาติ, ตตฺร เจ โส ภิกฺขุ ปุพฺเพ อปฺปวาริโต อุปสงฺกมิตฺวา จีวเร วิกปฺปํ อาปชฺเชยฺย “สาธุ วต มํ อายสฺมนฺโต อิเมหิ ปจฺเจกจีวรเจตาปเนหิ เอวรูปํ วา เอวรูปํ วา จีวรํ เจตาเปตฺวา อจฺฉาเทถ อุโภว สนฺตา เอเกนาติ กลฺยาณกมฺยตํ อุปาทาย, นิสฺสคฺคิยํ ปาจิตฺติยํ.</t>
   </si>
   <si>
-    <t>ภิกขุง ปะเนวะ อุททิสสะ อุภินนัง อัญญาตะกานัง คะหะปะตีนัง วา คะหะปะตานีนัง วา ปัจเจกะจีวะระเจตาปะนา อุปักขะฏา โหนติ “อิเมหิ มะยัง ปัจเจกะจีวะระเจตาปะเนหิ ปัจเจกะจีวะรานิ เจตาเปต๎วา อิตถันนามัง ภิกขุง จีวะเรหิ อัจฉาเทสสามาติ, ตัต๎ระ เจ โส ภิกขุ ปุพเพ อัปปะวาริโต อุปะสังกะมิต๎วา จีวะเร วิกัปปัง อาปัชเชยยะ "สาธุ วะตะ มัง อายัส๎มันโต อิเมหิ ปัจเจกะจีวะระเจตาปะเนหิ เอวะรูปัง วา เอวะรูปัง วา จีวะรัง เจตาเปต๎วา อัจฉาเทถะ อุโภวะ สันตา เอเกนาติ กัล๎ยาณะกัมยะตัง อุปาทายะ, นิสสัคคิยัง ปาจิตติยัง.</t>
+    <t>ภิกขุง ปะเนวะ อุททิสสะ อุภินนัง อัญญาตะกานัง คะหะปะตีนัง วา คะหะปะตานีนัง วา ปัจเจกะจีวะระเจตาปะนา อุปักขะฏา โหนติ “อิเมหิ มะยัง ปัจเจกะจีวะระเจตาปะเนหิ ปัจเจกะจีวะรานิ เจตาเปต๎วา อิตถันนามัง ภิกขุง จีวะเรหิ อัจฉาเทสสามาติ, ตัต๎ระ เจ โส ภิกขุ ปุพเพ อัปปะวาริโต อุปะสังกะมิต๎วา จีวะเร วิกัปปัง อาปัชเชยยะ "สาธุ วะตะ มัง อายัส๎มันโต อิเมหิ ปัจเจกะจีวะระเจตาปะเนหิ เอวะรูปัง วา เอวะรูปัง วา จีวะรัง เจตาเปต๎วา อัจฉาเทถะ อุโภวะ สันตา เอเกนาติ กัล๎ยาณะกัม๎ยะตัง อุปาทายะ, นิสสัคคิยัง ปาจิตติยัง.</t>
   </si>
   <si>
     <t>Bhikkhuṁ pan’eva uddissa ubhinnaṁ aññātakānaṁ gahapatīnaṁ vā gahapatānīnaṁ vā paccekacīvaracetāpanā upakkhaṭā honti “imehi mayaṁ paccekacīvara cetāpanehi paccekacīvarāni cetāpetvā itthannāmaṁ bhikkhuṁ cīvarehi acchādessāmā”ti. Tatra ce so bhikkhu pubbe appavārito upasaṅkamitvā cīvare vikappaṁ āpajjeyya, “Sādhu vata maṁ āyasmanto imehi paccekacīvaracetāpanehi evarūpaṁ vā evarūpaṁ vā cīvaraṁ cetāpetvā acchādetha ubho’va santā ekenā”ti kalyāṇakamyataṁ upādāya, nissaggiyaṁ pācittiyaṁ.</t>
@@ -1330,7 +1330,7 @@
         <rFont val="Arial"/>
         <color theme="1"/>
       </rPr>
-      <t xml:space="preserve">ภิกขุง ปะเนวะ อุททิสสะ ราชา วา ราชะโภคโค วา พราหมะโณ วา คะหะปะติโก วา ทูเตนะ จีวะระเจตาปะนัง ปะหิเณยยะ “อิมินา จีวะระเจตานาปะเนนะ จีวะรัง เจตาเปต๎วา อิตถันนามัง ภิกขุง จีวะเรนะ อัจฉาเทหีติ, โส เจ ทูโต ตัง ภิกขุง อุปะสังกะมิต๎วา เอวัง วะเทยยะ “อิทัง โข ภันเต อายัส๎มันตัง อุททิสสะ จีวะระเจตาปะนัง อาภะตัง, ปะฏิคคัณหาตุ อายัส๎มา จีวะระเจตาปะนันติ, เตนะ ภิกขุนา โส ทูโต เอวะมัสสะ วะจะนีโย “นะ โข มะยัง อาวุโส จีวะระเจตาปะนัง ปะฏิคคัณหามะ, จีวะรัญจะ โข มะยัง ปะฏิคคัณหามะ กาเลนะ กัปปิยันติ, โส เจ ทูโต ตัง ภิกขุง เอวัง วะเทยยะ “อัตถิ ปะนายัส๎มะโต โกจิ เวยยาวัจจะกะโรติ, จีวะรัตถิเกนะ ภิกขะเว ภิกขุนา เวยยาวัจจะกะโร นิททิสิตัพโพ อารามิโก วา อุปาสะโก วา “เอโส โข อาวุโส ภิกขูนัง เวยยาวัจจะกะโรติ, โส เจ ทูโต ตัง เวยยาวัจจะกะรัง สัญญาเปต๎วา ตัง ภิกขุง อุปะสังกะมิต๎วา เอวัง วะเทยยะ “ยัง โข ภันเต อายัส๎มา เวยยาวัจจะกะรัง นิททิสิ, สัญญัตโต โส มะยา, อุปะสังกะมะตุ อายัส๎มา กาเลนะ จีวะเรนะ ตัง อัจฉาเทสสะตีติ จีวะรัตถิเกนะ ภิกขะเว ภิกขุนา เวยยาวัจจะกะโร อุปะสังกะมิต๎วา ท๎วิตติกขัตตุง โจเทตัพโพ สาเรตัพโพ “อัตโถ เม อาวุโส จีวะเรนาติ, ท๎วิตติกขัตตุง โจทะยะมาโน สาระยะมาโน ตัง จีวะรัง อะภินิปผาเทยยะ, อิจเจตัง กุสะลัง, โน เจ อะภินิปผาเทยยะ, จะตุกขัตตุง ปัญจักขัตตุง ฉักขัตตุปะระมัง ตุณ๎หีภูเตนะ อุททิสสะ ฐาตัพพัง, จะตุกขัตตุง ปัญจักขัตตุง ฉักขัตตุปะระมัง ตุณ๎หีภูโต อุททิสสะ ติฏฐะมาโน ตัง จีวะรัง อะภินิปผาเทยยะ, อิจเจตัง กุสะลัง, โน เจ อะภินิปผาเทยยะ, ตะโต เจ อุตตะริง วายะมะมาโน ตัง จีวะรัง อะภินิปผาเทยยะ, นิสสัคคิยัง ปาจิตติยัง, โน เจ อะภินิปผาเทยยะ, ยะตัสสะ จีวะระเจตาปะนัง อาภะตัง, ตัตถะ สามัง วา คันตัพพัง, ทูโต วา ปาเหตัพโพ “ยัง โข ตุมเห อายัส๎มันโต ภิกขุง อุททิสสะ จีวะระเจตาปะนัง ปะหิณิตถะ, นะ ตันตัสสะ ภิกขุโน กิญจิ อัตถัง อะนุโภติ, ยุญชันตายัส๎มันโต สะกัง, มา โว สะกัง วินัสสีติ. อะยัง ตัตถะ สามีจิ.
+      <t xml:space="preserve">ภิกขุง ปะเนวะ อุททิสสะ ราชา วา ราชะโภคโค วา พ๎ราห๎มะโณ วา คะหะปะติโก วา ทูเตนะ จีวะระเจตาปะนัง ปะหิเณยยะ “อิมินา จีวะระเจตาปะเนนะ จีวะรัง เจตาเปต๎วา อิตถันนามัง ภิกขุง จีวะเรนะ อัจฉาเทหีติ, โส เจ ทูโต ตัง ภิกขุง อุปะสังกะมิต๎วา เอวัง วะเทยยะ “อิทัง โข ภันเต อายัส๎มันตัง อุททิสสะ จีวะระเจตาปะนัง อาภะตัง, ปะฏิคคัณหาตุ อายัส๎มา จีวะระเจตาปะนันติ, เตนะ ภิกขุนา โส ทูโต เอวะมัสสะ วะจะนีโย “นะ โข มะยัง อาวุโส จีวะระเจตาปะนัง ปะฏิคคัณหามะ, จีวะรัญจะ โข มะยัง ปะฏิคคัณหามะ กาเลนะ กัปปิยันติ, โส เจ ทูโต ตัง ภิกขุง เอวัง วะเทยยะ “อัตถิ ปะนายัส๎มะโต โกจิ เวยยาวัจจะกะโรติ, จีวะรัตถิเกนะ ภิกขะเว ภิกขุนา เวยยาวัจจะกะโร นิททิสิตัพโพ อารามิโก วา อุปาสะโก วา “เอโส โข อาวุโส ภิกขูนัง เวยยาวัจจะกะโรติ, โส เจ ทูโต ตัง เวยยาวัจจะกะรัง สัญญาเปต๎วา ตัง ภิกขุง อุปะสังกะมิต๎วา เอวัง วะเทยยะ “ยัง โข ภันเต อายัส๎มา เวยยาวัจจะกะรัง นิททิสิ, สัญญัตโต โส มะยา, อุปะสังกะมะตุ อายัส๎มา กาเลนะ จีวะเรนะ ตัง อัจฉาเทสสะตีติ จีวะรัตถิเกนะ ภิกขะเว ภิกขุนา เวยยาวัจจะกะโร อุปะสังกะมิต๎วา ท๎วิตติกขัตตุง โจเทตัพโพ สาเรตัพโพ “อัตโถ เม อาวุโส จีวะเรนาติ, ท๎วิตติกขัตตุง โจทะยะมาโน สาระยะมาโน ตัง จีวะรัง อะภินิปผาเทยยะ, อิจเจตัง กุสะลัง, โน เจ อะภินิปผาเทยยะ, จะตุกขัตตุง ปัญจักขัตตุง ฉักขัตตุปะระมัง ตุณ๎หีภูเตนะ อุททิสสะ ฐาตัพพัง, จะตุกขัตตุง ปัญจักขัตตุง ฉักขัตตุปะระมัง ตุณ๎หีภูโต อุททิสสะ ติฏฐะมาโน ตัง จีวะรัง อะภินิปผาเทยยะ, อิจเจตัง กุสะลัง, โน เจ อะภินิปผาเทยยะ, ตะโต เจ อุตตะริง วายะมะมาโน ตัง จีวะรัง อะภินิปผาเทยยะ, นิสสัคคิยัง ปาจิตติยัง, โน เจ อะภินิปผาเทยยะ, ยะตัสสะ จีวะระเจตาปะนัง อาภะตัง, ตัตถะ สามัง วา คันตัพพัง, ทูโต วา ปาเหตัพโพ “ยัง โข ตุม๎เห อายัส๎มันโต ภิกขุง อุททิสสะ จีวะระเจตาปะนัง ปะหิณิตถะ, นะ ตันตัสสะ ภิกขุโน กิญจิ อัตถัง อะนุโภติ, ยุญชันตายัส๎มันโต สะกัง, มา โว สะกัง วินัสสีติ. อะยัง ตัตถะ สามีจิ.
 </t>
     </r>
     <r>
@@ -1466,7 +1466,7 @@
     <t>โย ปน ภิกฺขุ ชาตรูปรชตํ อุคฺคณฺเหยฺย วา อุคฺคณฺหาเปยฺย วา อุปนิกฺขิตฺตํ วา สาทิเยยฺย, นิสฺสคฺคิยํ ปาจิตฺติยํ.</t>
   </si>
   <si>
-    <t>โย ปะนะ ภิกขุ ชาตะรูปะระชะตัง อุคคัณเหยยะ วา อุคคัณหาเปยยะ วา อุปะนิกขัตตัง วา สาทิเยยยะ, นิสสัคคิยัง ปาจิตติยัง.</t>
+    <t>โย ปะนะ ภิกขุ ชาตะรูปะระชะตัง อุคคัณเหยยะ วา อุคคัณหาเปยยะ วา อุปะนิกขิตตัง วา สาทิเยยยะ, นิสสัคคิยัง ปาจิตติยัง.</t>
   </si>
   <si>
     <t>Yo pana bhikkhu jātarūparajataṁ uggaṇheyya vā uggaṇhāpeyya vā upanikkhittaṁ vā sādiyeyya, nissaggiyaṁ pācittiyaṁ.</t>
@@ -1571,7 +1571,7 @@
     <t>๒๑. พึงทรงอติเรกบาตรไว้ได้ ๑๐ วันเป็นอย่างยิ่ง ภิกษุให้ล่วงกำหนดนั้นไปเป็นนิสสัคคิยปาจิตตีย์.</t>
   </si>
   <si>
-    <t>โย ปน ภิกฺขุ อูนปญฺจพนฺธเนน ปตฺเตน อญฺญํ นวํ ปตฺตํ เจตาเปยฺย, นิสฺสคฺคิยํ ปาจิตฺติยํ. เตน ภิกฺขุนา โส ปตฺโต ภิกฺขุปริสาย นิสฺสชฺชิตพฺโพ; โย จ ตสฺสา ภิกฺขุปริสาย ปตฺตปริยนฺโต, โส จ ตสฺส ภิกฺขุโน ปทาตพฺโพ“อยนฺเต ภิกฺขุ ปตฺโต, ยาว เภทนาย ธาเรตพฺโพติ: อยํ ตตฺถ สามีจิ.</t>
+    <t>โย ปน ภิกฺขุ อูนปญฺจพนฺธเนน ปตฺเตน อญฺญํ นวํ ปตฺตํ เจตาเปยฺย, นิสฺสคฺคิยํ ปาจิตฺติยํ. เตน ภิกฺขุนา โส ปตฺโต ภิกฺขุปริสาย นิสฺสชฺชิตพฺโพ; โย จ ตสฺสา ภิกฺขุปริสาย ปตฺตปริยนฺโต, โส จ ตสฺส ภิกฺขุโน ปทาตพฺโพ “อยนฺเต ภิกฺขุ ปตฺโต, ยาว เภทนาย ธาเรตพฺโพติ: อยํ ตตฺถ สามีจิ.</t>
   </si>
   <si>
     <t>โย ปะนะ ภิกขุ อูนะปัญจะพันธะเนนะ ปัตเตนะ อัญญัง นะวัง ปัตตัง เจตาเปยยะ, นิสสัคคิยัง ปาจิตติยัง. เตนะ ภิกขุนา โส ปัตโต ภิกขุปะริสายะ นิสสัชชิตัพโพ, โย จะ ตัสสา ภิกขุปะริสายะ ปัตตะปะริยันโต, โส จะ ตัสสะ ภิกขุโน ปะทาตัพโพ “อะยันเต ภิกขุ ปัตโต, ยาวะ เภทะนายะ ธาเรตัพโพติ. อะยัง ตัตถะ สามีจิ.</t>
@@ -1598,7 +1598,7 @@
     <t>“มาโส เสโส คิมฺหานนฺติ ภิกฺขุนา วสฺสิกสาฏิกจีวรํ ปริเยสิตพฺพํ, “อฑฺฒมาโส เสโส คิมฺหานนฺติ กตฺวา นิวาเสตพฺพํ; “โอเรน เจ มาโส เสโส คิมฺหานนฺติ วสฺสิกสาฏิกจีวรํ ปริเยเสยฺย. “โอเรนฑฺฒมาโส เสโส คิมฺหานนฺติ กตฺวา นิวาเสยฺย; นิสฺสคฺคิยํ ปาจิตฺติยํ.</t>
   </si>
   <si>
-    <t>“มาโส เสโส คิมหานันติ ภิกขุนา วัสสิกะสาฏิกะจีวะรัง ปะริเยสิตัพพัง, “อัฑฒะมาโส เสโส คิมหานันติ กัต๎วา นิวาเสตัพพัง, “โอเรนะ เจ มาโส เสโส คิมหานันติ วัสสิกะสาฏิกะจีวะรัง ปะริเยเสยยะ. “โอเรนัฑฒะมาโส เสโส คิมหานันติ กัต๎วา นิวาเสยยะ, นิสสัคคิยัง ปาจิตติยัง.</t>
+    <t>“มาโส เสโส คิม๎หานันติ ภิกขุนา วัสสิกะสาฏิกะจีวะรัง ปะริเยสิตัพพัง, “อัฑฒะมาโส เสโส คิม๎หานันติ กัต๎วา นิวาเสตัพพัง, “โอเรนะ เจ มาโส เสโส คิม๎หานันติ วัสสิกะสาฏิกะจีวะรัง ปะริเยเสยยะ. “โอเรนัฑฒะมาโส เสโส คิม๎หานันติ กัต๎วา นิวาเสยยะ, นิสสัคคิยัง ปาจิตติยัง.</t>
   </si>
   <si>
     <t>Māso seso gimhānan’ti bhikkhunā vassikasāṭikacīvaraṁ pariyesitabbaṁ, aḍḍhamāso seso gimhānan’ti, katvā nivāsetabbaṁ. Orena ce māso seso gimhānan’ti, vassikasāṭikacīvaraṁ pariyeseyya, oren’aḍḍhamāso seso gimhānan’ti katvā nivāseyya, nissaggiyaṁ pācittiyaṁ.</t>
@@ -1619,7 +1619,7 @@
     <t>๒๕. อนึ่ง ภิกษุใด ให้จีวรแก่ภิกษุเองแล้ว โกรธน้อยใจชิงเอามาก็ดี ให้ชิงเอามาก็ดี เป็นนิสสัคคิยปาจิตตีย์</t>
   </si>
   <si>
-    <t>โย ปน ภิกฺขุ สามํ สุตฺตํ วิญฺญาเปตฺวา ตนฺต วาเยหิ จีวรํ วายาเปยฺย, นิสฺสคฺคิยํ ปาจิตฺติยํ.</t>
+    <t>โย ปน ภิกฺขุ สามํ สุตฺตํ วิญฺญาเปตฺวา ตนฺตวาเยหิ จีวรํ วายาเปยฺย, นิสฺสคฺคิยํ ปาจิตฺติยํ.</t>
   </si>
   <si>
     <t>โย ปะนะ ภิกขุ สามัง สุตตัง วิญญาเปต๎วา ตันตะวาเยหิ จีวะรัง วายาเปยยะ, นิสสัคคิยัง ปาจิตติยัง.</t>
@@ -1631,7 +1631,7 @@
     <t>๒๖. อนึ่ง ภิกษุใดขอด้ายมาเองแล้ว ยังช่างหูกให้ทอจีวร เป็น นิสสัคคิยปาจิตตีย์</t>
   </si>
   <si>
-    <t>ภิกฺขุํ ปเนว อุทฺทิสฺส อญฺญาตโก คหปติ วา คหปตานี วา ตนฺตวาเยหิ จีวรํ วายาเปยฺย, ตตฺร เจ โส ภิกฺขุ ปุพฺเพ อปฺปวาริโต ตนฺตวาเย อุปสงฺกมิตฺวา จีวเร วิกปฺปํ อาปชฺเชยฺย “อิทํ โข อาวุโส จีวรํ มํ อุทฺทิสฺส วียติ, อายตญฺจ กโรถ, วิตฺถตญฺจ อปฺปิตญฺจ สุวิตญฺจ1 สุปวายิตญฺจ สุวิเลกฺขิตญฺจ2 สุวิตจฺฉิตญฺจ กโรถ; อปฺเปว นาม มยมฺปิ อายสฺมนฺตานํ กิญฺจิมตฺตํ อนุปทชฺเชยฺยามาติ, เอวญฺจ โส ภิกฺขุ วตฺวา กิญฺจิมตฺตํ อนุปทชฺเชยฺย อนฺตมโส ปิณฺฑปาตมตฺตมฺปิ, นิสฺสคฺคิยํ ปาจิตฺติยํ.</t>
+    <t>ภิกฺขุํ ปเนว อุทฺทิสฺส อญฺญาตโก คหปติ วา คหปตานี วา ตนฺตวาเยหิ จีวรํ วายาเปยฺย, ตตฺร เจ โส ภิกฺขุ ปุพฺเพ อปฺปวาริโต ตนฺตวาเย อุปสงฺกมิตฺวา จีวเร วิกปฺปํ อาปชฺเชยฺย “อิทํ โข อาวุโส จีวรํ มํ อุทฺทิสฺส วียติ, อายตญฺจ กโรถ, วิตฺถตญฺจ อปฺปิตญฺจ สุวิตญฺจ สุปวายิตญฺจ สุวิเลกฺขิตญฺจ สุวิตจฺฉิตญฺจ กโรถ; อปฺเปว นาม มยมฺปิ อายสฺมนฺตานํ กิญฺจิมตฺตํ อนุปทชฺเชยฺยามาติ, เอวญฺจ โส ภิกฺขุ วตฺวา กิญฺจิมตฺตํ อนุปทชฺเชยฺย อนฺตมโส ปิณฺฑปาตมตฺตมฺปิ, นิสฺสคฺคิยํ ปาจิตฺติยํ.</t>
   </si>
   <si>
     <t>ภิกขุง ปะเนวะ อุททิสสะ อัญญาตะโก คะหะปะติ วา คะหะปะตานี วา ตันตะวาเยหิ จีวะรัง วายาเปยยะ, ตัต๎ระ เจ โส ภิกขุ ปุพเพ อัปปะวาริโต ตันตะวาเย อุปะสังกะมิต๎วา จีวะเร วิกัปปัง อาปัชเชยยะ “อิทัง โข อาวุโส จีวะรัง มัง อุททิสสะ วียะติ, อายะตัญจะ กะโรถะ, วิตถะตัญจะ อัปปิตัญจะ สุวิตัญจะ สุปะวายิตัญจะ สุวิเลกขิตัญจะ สุวิตัจฉิตัญจะ กะโรถะ, อัปเปวะ นามะ มะยัมปิ อายัส๎มันตานัง กิญจิมัตตัง อะนุปะทัชเชยยามาติ, เอวัญจะ โส ภิกขุ วัต๎วา กิญจิมัตตัง อะนุปะทัชเชยยะ อันตะมะโส ปิณฑะปาตะมัตตัมปิ, นิสสัคคิยัง ปาจิตติยัง.</t>
@@ -2135,7 +2135,7 @@
     <t>๑๔. อนึ่ง ภิกษุใด วางไว้แล้วก็ดี ให้วางไว้แล้วก็ดี ซึ่งเตียงก็ดี ตั่งก็ดี ฟูกก็ดีเก้าอี้ก็ดี อันเป็นของสงฆ์ในที่แจ้ง.เมื่อหลีกไป ไม่เก็บก็ดี ไม่ให้เก็บก็ดี ซึ่งเสนาสนะที่วางไว้นั้น หรือไม่บอกสั่ง ไปเสีย เป็นปาจิตตีย์.</t>
   </si>
   <si>
-    <t>โย ปน ภิกฺขุ สงฺฆิเก วิหาเร เสยฺยํ สนฺถริตฺวา วา สนฺถราเปตฺวา วา ตํ ปกกฺมนฺโต เนว อุทฺธเรยฺย น อุทฺธราเปยฺย อนาปุจฺฉํ วา คจฺเฉยฺย, ปาจิตฺติยํ.</t>
+    <t>โย ปน ภิกฺขุ สงฺฆิเก วิหาเร เสยฺยํ สนฺถริตฺวา วา สนฺถราเปตฺวา วา ตํ ปกฺกมนฺโต เนว อุทฺธเรยฺย น อุทฺธราเปยฺย อนาปุจฺฉํ วา คจฺเฉยฺย, ปาจิตฺติยํ.</t>
   </si>
   <si>
     <t>โย ปะนะ ภิกขุ สังฆิเก วิหาเร เสยยัง สันถะริต๎วา วา สันถะราเปต๎วา วา ตัง ปักกะมันโต เนวะ อุทธะเรยยะ นะ อุทธะราเปยยะ อะนาปุจฉัง วา คัจเฉยยะ, ปาจิตติยัง.</t>
@@ -2578,7 +2578,7 @@
         <rFont val="Arial"/>
         <color theme="1"/>
       </rPr>
-      <t xml:space="preserve">โย ปะนะ ภิกขุ อะทินนัง มุขะท๎วารัง อาหารัง อาหะเรยยะ อัญญัต๎ระ อุทะกะทันตะโปณา, ปาจิตติยัง.
+      <t xml:space="preserve">โย ปะนะ ภิกขุ อะทินนัง มุขัท๎วารัง อาหารัง อาหะเรยยะ อัญญัต๎ระ อุทะกะทันตะโปณา, ปาจิตติยัง.
 </t>
     </r>
     <r>
@@ -2642,7 +2642,7 @@
     <t>โย ปน ภิกฺขุ ภิกฺขุํ เอวํ วเทยฺย “เอหาวุโส คามํ วา นิคมํ วา ปิณฺฑาย ปวิสิสฺสามาติ. ตสฺส ทาเปตฺวา วา อทาเปตฺวา วา อุยฺโยเชยฺย “คจฺฉาวุโส, น เม ตยา สทฺธึ กถา วา นิสชฺชา วา ผาสุ โหติ, เอกกสฺส เม กถา วา นิสชฺชา วา ผาสุ โหตีติ, เอตเทว ปจฺจยํ กริตฺวา อนญฺญํ , ปาจิตฺติยํ.</t>
   </si>
   <si>
-    <t>โย ปะนะ ภิกขุ ภิกขุง (เอวัง วะเทยยะ) “เอหาวุโส คามัง วา นิคะมัง วา ปิณฑายะ ปะวิสิสสามาติ. ตัสสะ ทาเปต๎วา วา อะทาเปต๎วา วา อุยโยเชยยะ “คัจฉาวุโส, นะ เม ตะยา สัทธิง กะถา วา นิสัชชา วา ผาสุ โหติ, เอกะกัสสะ เม กะถา วา นิสัชชา วา ผาสุ โหตีติ, เอตะเทวะ ปัจจะยัง กะริต๎วา อะนัญญัง, ปาจิตติยัง.</t>
+    <t>โย ปะนะ ภิกขุ ภิกขุง เอวัง วะเทยยะ “เอหาวุโส คามัง วา นิคะมัง วา ปิณฑายะ ปะวิสิสสามาติ. ตัสสะ ทาเปต๎วา วา อะทาเปต๎วา วา อุยโยเชยยะ “คัจฉาวุโส, นะ เม ตะยา สัทธิง กะถา วา นิสัชชา วา ผาสุ โหติ, เอกะกัสสะ เม กะถา วา นิสัชชา วา ผาสุ โหตีติ, เอตะเทวะ ปัจจะยัง กะริต๎วา อะนัญญัง, ปาจิตติยัง.</t>
   </si>
   <si>
     <t>Yo pana bhikkhu bhikkhuṁ evaṁ vadeyya, “Eh’āvuso gāmaṁ vā nigamaṁ vā piṇḍaya pavisissāmāti. Tassa dāpetvā vā adāpetvā vā uyyojeyya “gacch’ āvuso, na me tayā saddhiṁ kathā vā nisajjā vā phāsu hoti, ekakassa me kathā vā nisajjā vā phāsu hotī”ti. Etad’eva paccayaṁ karitvā anaññaṁ, pācittiyaṁ.</t>
@@ -2882,7 +2882,7 @@
     <t>โย ปน ภิกฺขุ โอเรนฑฺฒมาสํ นฺหาเยยฺย อญฺญตฺร สมยา, ปาจิตฺติยํ. ตตฺถายํ สมโย: ทิยฑฺโฒ มาโส เสโส คิมฺหานนฺติ วสฺสานสฺส ปฐโม มาโส อิจฺเจเต อฑฺฒเตยฺยมาสา อุณฺหสมโย ปริฬาหสมโย คิลานสมโย กมฺมสมโย อทฺธานคมนสมโย วาตวุฏฺฐิสมโย. อยํ ตตฺถ สมโย.</t>
   </si>
   <si>
-    <t>โย ปะนะ ภิกขุ โอเรนัฑฒะมาสัง นะหาเยยยะ อัญญัต๎ระ สะมะยา, ปาจิตติยัง. ตัตถายัง สะมะโย. ทิยัฑโฒ มาโส เสโส คิมหานันติ วัสสานัสสะ ปะฐะโม มาโส อิจเจเต อัฑฒะเตยยะมาสา อุณหะสะมะโย ปะริฬาหะสะมะโย คิลานะสะมะโย กัมมะสะมะโย อัทธานะคะมะนะสะมะโย วาตะวุฏฐิสะมะโย, อะยัง ตัตถะ สะมะโย.</t>
+    <t>โย ปะนะ ภิกขุ โอเรนัฑฒะมาสัง น๎หาเยยยะ อัญญัต๎ระ สะมะยา, ปาจิตติยัง. ตัตถายัง สะมะโย. ทิยัฑโฒ มาโส เสโส คิม๎หานันติ วัสสานัสสะ ปะฐะโม มาโส อิจเจเต อัฑฒะเตยยะมาสา อุณหะสะมะโย ปะริฬาหะสะมะโย คิลานะสะมะโย กัมมะสะมะโย อัทธานะคะมะนะสะมะโย วาตะวุฏฐิสะมะโย, อะยัง ตัตถะ สะมะโย.</t>
   </si>
   <si>
     <t>Yo pana bhikkhu orenaḍḍhamāsaṁ nhāyeyya, aññatra samayā, pācittiyaṁ. Tatthāyaṁ samayo. Diyaḍḍho māso seso gimhānan’ti, vassānassa, paṭhamo māso icc’ete aḍḍhateyyamāsā uṇhasamayo, pariḷāhasamayo, gilānasamayo, kammasamayo, addhānagamanasamayo, vātavuṭṭhisamayo, ayaṁ tattha samayo.</t>
@@ -2894,7 +2894,7 @@
     <t>นวมฺปน ภิกฺขุนา จีวรลาเภน ติณฺณํ ทุพฺพณฺณกรณานํ อญฺญตรํ ทุพฺพณฺณกรณํ อาทาตพฺพํ นีลํ วา กทฺทมํ วา กาฬสามํ วา, อนาทา เจ ภิกฺขุ ติณฺณํ ทุพฺพณฺณกรณานํ อญฺญตรํ ทุพฺพณฺณกรณํ นวํ จีวรํ ปริภุญฺเชยฺย, ปาจิตฺติยํ.</t>
   </si>
   <si>
-    <t>นะวัมปะนะ ภิกขุนา จีวะระลาเภนะ ติณณัง ทุพพัณณะกะระณานัง อัญญะตะรัง ทุพพัณณะกะระณัง อา ทาตัพพัง นีลัง วา กัททะมัง วา กาฬะสามัง วา, อะนาทา เจ ภิกขุ ติณณัง ทุพพัณณะกะระณานัง อัญญะตะรัง ทุพพัณณะ กะระณัง นะวัง จีวะรัง ปะริภุญเชยยะ, ปาจิต ติยัง.</t>
+    <t>นะวัมปะนะ ภิกขุนา จีวะระลาเภนะ ติณณัง ทุพพัณณะกะระณานัง อัญญะตะรัง ทุพพัณณะกะระณัง อาทาตัพพัง นีลัง วา กัททะมัง วา กาฬะสามัง วา, อะนาทา เจ ภิกขุ ติณณัง ทุพพัณณะกะระณานัง อัญญะตะรัง ทุพพัณณะกะระณัง นะวัง จีวะรัง ปะริภุญเชยยะ, ปาจิตติยัง.</t>
   </si>
   <si>
     <t>Navaṁ pana bhikkhunā cīvaralābhena tiṇṇaṁ dubbaṇṇakaraṇānaṁ aññataraṁ dubbaṇṇakaraṇaṁ ādātabbaṁ nīlaṁ vā kaddamaṁ vā kālasāmaṁ vā anādā ce bhikkhu tiṇṇaṁ dubbaṇṇakaraṇānaṁ aññataraṁ dubbaṇṇakaraṇaṁ navaṁ cīvaraṁ paribhuñjeyya, pācittiyaṁ.</t>
@@ -3011,7 +3011,7 @@
     <t>๖๒. อนึ่ง ภิกษุใดรู้อยู่บริโภคน้ำมีตัวสัตว์ เป็นปาจิตตีย์.</t>
   </si>
   <si>
-    <t>โย ปน ภิกฺขุ ชานํ ยถาธมฺมํ นีห1ตาธิกรณํ ปุนกมฺมาย อุกฺโกเฏยฺย, ปาจิตฺติยํ.</t>
+    <t>โย ปน ภิกฺขุ ชานํ ยถาธมฺมํ นีหตาธิกรณํ ปุนกมฺมาย อุกฺโกเฏยฺย, ปาจิตฺติยํ.</t>
   </si>
   <si>
     <t>โย ปะนะ ภิกขุ ชานัง ยะถาธัมมัง นีหะตาธิกะระณัง ปุนะกัมมายะ อุกโกเฏยยะ, ปาจิตติยัง.</t>
@@ -3071,10 +3071,10 @@
     <t>๖๗. อนึ่ง ภิกษุใด ชักชวนแล้วเดินทางไกลสายเดียวกันกับมาตุคาม โดยที่สุดแม้สิ้นระยะบ้านหนึ่ง เป็นปาจิตตีย์.</t>
   </si>
   <si>
-    <t>โย ปน ภิกฺขุ เอวํ วเทยฺย “ตถาหํ ภควตา ธมฺมํ เทสิตํ อาชานามิ; ยถา เยเม อนฺตรายิกา ธมฺมา วุตฺตา ภควตา, เต ปฏิเสวโต นาลํ อนฺตรายายาติ, โส ภิกฺขุ ภิกฺขูหิ เอวมสฺส วจนีโย “มา อายสฺมา เอวํ อวจ, มา ภควนฺตํ อพฺภาจิกฺขิ; น หิ สาธุ ภควโต อพฺภกฺขานํ, น หิ ภควา เอวํ วเทยฺย; อเนกปริยาเยน อาวุโส อนฺตรายิกา ธมฺมา1 วุตฺตา ภควตา, อลญฺจ ปน เต ปฏิเสวโต อนฺตรายายาติ; เอวญฺจ โส ภิกฺขุ ภิกฺขูหิ วุจฺจมาโน ตเถว ปคฺคณฺเหยฺย, โส ภิกฺขุ ภิกฺขูหิ ยาวตติยํ สมนุภาสิตพฺโพ ตสฺส ปฏินิสฺสคฺคาย; ยาวตติยญฺเจ สมนุภาสิยมาโน ตํ ปฏินิสฺสชฺเชยฺย, อิจฺเจตํ กุสลํ, โน เจ ปฏินิสฺสชฺเชยฺย, ปาจิตฺติยํ.</t>
-  </si>
-  <si>
-    <t>โย ปะนะ ภิกขุ เอวัง วะเทยยะ “ตะถาหัง ภะคะวะตา ธัมมัง เทสิตัง อาชานามิ. ยะถา เยเม อันตะรายิกา ธัมมา วุตตา ภะคะวะตา เต ปะฏิเสวะโต นาลัง อันตะรายายาติ, โส ภิกขุ ภิกขูหิ เอวะมัสสะ วะจะนีโย “มา อายัส๎มา เอวัง อะวะจะ, มา ภะคะวันตัง อัพภาจิกขิ, นะ หิ สาธุ ภะคะวะโต อัพภักขานัง, นะ หิ ภะคะวา เอวัง วะเทยยะ, อะเนกะปะริยาเยนะ อาวุโส อันตะรายิกา ธัมมา วุตตา ภะคะวะตา , อะลัญจะ ปะนะ เต ปะฏิเสวะโต อันตะรายายาติ, เอวัญจะ โส ภิกขุ ภิกขูหิ วุจจะมาโน ตะเถวะ ปัคคัณเหยยะ, โส ภิกขุ ภิกขูหิ ยาวะตะติยัง สะมะนุภาสิตัพโพ ตัสสะ ปะฏินิสสัคคายะ, ยาวะ ตะติยัญเจ สะมะนุภาสิยะมาโน ตัง ปะฏินิสสัชเชยยะ, อิจเจตัง, กุสะลัง, โน เจ ปะฏินิสสัชเชยยะ, ปาจิตติยัง.</t>
+    <t>โย ปน ภิกฺขุ เอวํ วเทยฺย “ตถาหํ ภควตา ธมฺมํ เทสิตํ อาชานามิ; ยถา เยเม อนฺตรายิกา ธมฺมา วุตฺตา ภควตา, เต ปฏิเสวโต นาลํ อนฺตรายายาติ, โส ภิกฺขุ ภิกฺขูหิ เอวมสฺส วจนีโย “มา อายสฺมา เอวํ อวจ, มา ภควนฺตํ อพฺภาจิกฺขิ; น หิ สาธุ ภควโต อพฺภกฺขานํ, น หิ ภควา เอวํ วเทยฺย; อเนกปริยาเยน อาวุโส อนฺตรายิกา ธมฺมา วุตฺตา ภควตา, อลญฺจ ปน เต ปฏิเสวโต อนฺตรายายาติ; เอวญฺจ โส ภิกฺขุ ภิกฺขูหิ วุจฺจมาโน ตเถว ปคฺคณฺเหยฺย, โส ภิกฺขุ ภิกฺขูหิ ยาวตติยํ สมนุภาสิตพฺโพ ตสฺส ปฏินิสฺสคฺคาย; ยาวตติยญฺเจ สมนุภาสิยมาโน ตํ ปฏินิสฺสชฺเชยฺย, อิจฺเจตํ กุสลํ, โน เจ ปฏินิสฺสชฺเชยฺย, ปาจิตฺติยํ.</t>
+  </si>
+  <si>
+    <t>โย ปะนะ ภิกขุ เอวัง วะเทยยะ “ตะถาหัง ภะคะวะตา ธัมมัง เทสิตัง อาชานามิ. ยะถา เยเม อันตะรายิกา ธัมมา วุตตา ภะคะวะตา เต ปะฏิเสวะโต นาลัง อันตะรายายาติ, โส ภิกขุ ภิกขูหิ เอวะมัสสะ วะจะนีโย “มา อายัส๎มา เอวัง อะวะจะ, มา ภะคะวันตัง อัพภาจิกขิ, นะ หิ สาธุ ภะคะวะโต อัพภักขานัง, นะ หิ ภะคะวา เอวัง วะเทยยะ, อะเนกะปะริยาเยนะ อาวุโส อันตะรายิกา ธัมมา วุตตา ภะคะวะตา , อะลัญจะ ปะนะ เต ปะฏิเสวะโต อันตะรายายาติ, เอวัญจะ โส ภิกขุ ภิกขูหิ วุจจะมาโน ตะเถวะ ปัคคัณเหยยะ, โส ภิกขุ ภิกขูหิ ยาวะตะติยัง สะมะนุภาสิตัพโพ ตัสสะ ปะฏินิสสัคคายะ, ยาวะตะติยัญเจ สะมะนุภาสิยะมาโน ตัง ปะฏินิสสัชเชยยะ, อิจเจตัง, กุสะลัง, โน เจ ปะฏินิสสัชเชยยะ, ปาจิตติยัง.</t>
   </si>
   <si>
     <t>Yo pana bhikkhu evaṁ vadeyya, “tathāhaṁ bhagavatā dhammaṁ desitaṁ ājānāmi. Yathā ye’me antarāyikā dhammā vuttā bhagavatā, te paṭisevato nālaṁ antarāyāyā” ti. So bhikkhu bhikkhūhi evam’assa vacanīyo, “mā āyasmā evaṁ avaca. Mā bhagavantaṁ abbhācikkhi, na hi sādhu bhagavato abbhakkhānaṁ na hi bhagavā evaṁ vadeyya. Anekapariyāyena āvuso antarāyikā dhammā vuttā bhagavatā alañca pana te paṭisevato antarāyāyā” ti: Evañca so bhikkhu bhikkhūhi vuccamāno tath’eva paggaṇheyya. So bhikkhu bhikkhūhi yāvatatiyaṁ samanubhāsitabbo tassa paṭinissaggāya, yāvatatiyañce samanubhāsiyamāno taṁ paṭinissajjeyya, icc’etaṁ kusalaṁ: No ce paṭinissajjeyya, pācittiyaṁ.</t>
@@ -3194,7 +3194,7 @@
     <t>โย ปน ภิกฺขุ อนฺวฑฺฒมาสํ ปาฏิโมกฺเข อุทฺทิสฺสมาเน เอวํ วเทยฺย “อิทาเนว โข อหํ อาชานามิ ‘อยมฺปิ กิร ธมฺโม สุตฺตาคโต สุตฺตปริยาปนฺโน อนฺวฑฺฒมาสํ อุทฺเทสํ อาคจฺฉตีติ; ตญฺเจ ภิกฺขุํ อญฺเญ ภิกฺขู ชาเนยฺยุํ “นิสินฺนปุพฺพํ อิมินา ภิกฺขุนา ทฺวิตฺติกฺขตฺตุํ ปาฏิโมกฺเข อุทฺทิสฺสมาเน โก ปน วาโท ภิยฺโยติ, น จ ตสฺส ภิกฺขุโน อญฺญาณเกน มุตฺติ อตฺถิ; ยญฺจ ตตฺถ อาปตฺตึ อาปนฺโน, ตญฺจ ยถาธมฺโม กาเรตพฺโพ; อุตฺตริญฺจสฺส โมโห อาโรเปตพฺโพ “ตสฺส เต อาวุโส อลาภา, ตสฺส เต ทุลฺลทฺธํ; ยํ ตฺวํ ปาฏิโมกฺเข อุทฺทิสฺสมาเน น สาธุกํ อฏฺฐิกตฺวา มนสิกโรสีติ; อิทํ ตสฺมึ โมหนเก, ปาจิตฺติยํ.</t>
   </si>
   <si>
-    <t>โย ปะนะ ภิกขุ อัน๎วัฑฒะมาสัง ปาฏิโมกเข อุททิสสะมาเน เอวัง วะเทยยะ “อิทาเนวะ โข อะหัง อาชานามิ “อะยัมปิ กิระ ธัมโม สุตตาคะโต สุตตะปะริยาปันโน อัน๎วัฑฒะมาสัง อุทเทสัง อาคัจฉะตีติ, ตัญเจ ภิกขุง อัญเญ ภิกขู ชาเนยยุง “นิสินนะปุพพัง อิมินา ภิกขุนา ท๎วิตติกขัตตุง ปาฏิโมกเข อุททิสสะมาเน โก ปะนะ วาโท ภิยโยติ, นะ จะ ตัสสะ ภิกขุโน อัญญาณะเกนะ มุตติ อัตถิ, ยัญจะ ตัตถะ อาปัตติง อาปันโน, ตัญจะ ยะถา ธัมโม กาเรตัพโพ, อุตตะริญจัสสะ โมโห อาโรเปตัพโพ “ตัสสะ เต อาวุโส อะลาภา, ตัสสะ เต ทุลลัทธัง, ยัง ต๎วัง ปาฏิโมกเข อุททิสสะมาเน นะ สาธุกัง อัฏฐิกัต๎วา มะนะสิกะโรสีติ, อิทัง ตัส๎มิง โมหะนะเก ปาจิตติยัง.</t>
+    <t>โย ปะนะ ภิกขุ อัน๎วัฑฒะมาสัง ปาฏิโมกเข อุททิสสะมาเน เอวัง วะเทยยะ “อิทาเนวะ โข อะหัง อาชานามิ “อะยัมปิ กิระ ธัมโม สุตตาคะโต สุตตะปะริยาปันโน อัน๎วัฑฒะมาสัง อุทเทสัง อาคัจฉะตีติ, ตัญเจ ภิกขุง อัญเญ ภิกขู ชาเนยยุง “นิสินนะปุพพัง อิมินา ภิกขุนา ท๎วิตติกขัตตุง ปาฏิโมกเข อุททิสสะมาเน โก ปะนะ วาโท ภิยโยติ, นะ จะ ตัสสะ ภิกขุโน อัญญาณะเกนะ มุตติ อัตถิ, ยัญจะ ตัตถะ อาปัตติง อาปันโน, ตัญจะ ยะถาธัมโม กาเรตัพโพ, อุตตะริญจัสสะ โมโห อาโรเปตัพโพ “ตัสสะ เต อาวุโส อะลาภา, ตัสสะ เต ทุลลัทธัง, ยัง ต๎วัง ปาฏิโมกเข อุททิสสะมาเน นะ สาธุกัง อัฏฐิกัต๎วา มะนะสิกะโรสีติ, อิทัง ตัส๎มิง โมหะนะเก ปาจิตติยัง.</t>
   </si>
   <si>
     <t>Yo pana bhikkhu anvaḍḍhamāsaṁ pāṭimokkhe uddissamāne evaṁ vadeyya, “Idān’eva kho ahaṁ ājānāmi, ayam’pi kira dhammo suttāgato suttapariyāpanno anvaḍḍhamāsaṁ uddesaṁ āgacchatī”ti. Tañce bhikkhuṁ aññe bhikkhū jāneyyuṁ, “nisinnapubbaṁ iminā bhikkhunā dvittikkhattuṁ pātimokkhe uddissamāne ko pana vādo bhiyyo”ti, na ca tassa bhikkhuno aññāṇnakena mutti atthi: Yañca tattha āpattiṁ āpanno, tañca yathādhammo kāretabbo uttariñc’assa moho āropetabbo, “tassa te āvuso alābhā, tassa te dulladdhaṁ. Yaṁ tvaṁ pāṭimokkhe uddissamāne na sādhukaṁ aṭṭhikatvā manasikarosī”ti. Idaṁ tasmiṁ mohanake, pācittiyaṁ.</t>
@@ -3263,7 +3263,7 @@
     <t>๗๘. อนึ่ง ภิกษุใด เมื่อภิกษุทั้งหลาย เกิดหมางกัน เกิดทะเลาะกัน ถึงการวิวาทกัน ยืนแอบฟัง ด้วยหมายว่า "จักได้ฟังคำที่เธอพูดกัน"  ทำความหมายอย่างนี้เท่านั้นแล ให้เป็นปัจจัยหาใช่อย่างอื่นไม่ เป็นปาจิตตีย์.</t>
   </si>
   <si>
-    <t>โย ปน ภิกฺขุ ธมฺมิกานํ กมฺมานํ ฉนฺทํ ทตฺวา ปจฺฉา ขิยฺยนธมฺมํ1 อาปชฺเชยฺย, ปาจิตฺติยํ.</t>
+    <t>โย ปน ภิกฺขุ ธมฺมิกานํ กมฺมานํ ฉนฺทํ ทตฺวา ปจฺฉา ขิยฺยนธมฺมํ อาปชฺเชยฺย, ปาจิตฺติยํ.</t>
   </si>
   <si>
     <t>โย ปะนะ ภิกขุ ธัมมิกานัง กัมมานัง ฉันทัง ทัต๎วา ปัจฉา ขิยยะนะธัมมัง อาปัชเชยยะ, ปาจิตติยัง.</t>
@@ -3734,7 +3734,7 @@
     <t>ภิกฺขู ปเนว กุเลสุ นิมนฺติตา ภุญฺชนฺติ, ตตฺร เจ ภิกฺขุนี โวสาสมานรูปา ฐิตา โหติ “อิธ สูปํ เทถ, อิธ โอทนํ เทถาติ, เตหิ ภิกฺขูหิ สา ภิกฺขุนี อปสาเทตพฺพา “อปสกฺก ตาว ภคินิ, ยาว ภิกฺขู ภุญฺชนฺตีติ: เอกสฺสปิ เจ ภิกฺขุโน นปฺปฏิภาเสยฺย ตํ ภิกฺขุนึ อปสาเทตุํ “อปสกฺก ตาว ภคินิ, ยาว ภิกฺขู ภุญฺชนฺตีติ, ปฏิเทเสตพฺพํ เตหิ ภิกฺขูหิ “คารยฺหํ อาวุโส ธมฺมํ อาปชฺชิมฺหา อสปฺปายํ ปาฏิเทสนียํ, ตํ ปฏิเทเสมาติ.</t>
   </si>
   <si>
-    <t>ภิกขู ปะเนวะ กุเลสุ นิมันติตา ภุญชันติ, ตัต๎ระ เจ ภิกขุนี โวสาสะมานะรูปา ฐิตา โหติ “อิธะ สูปัง เทถะ, อิธะ โอทะนัง เทถาติ, เตหิ ภิกขูหิ สา ภิกขุนี อะปะสาเทตัพพา “อะปะสักกะ ตาวะ ภะคินิ, ยาวะ ภิกขู ภุญชันตีติ, เอกัสสะปิ เจ ภิกขุโน นัปปะฏิภาเสยยะ ตัง ภิกขุนิง อะปะสาเทตุง “อะปะสักกะ ตาวะ ภะคินิ, ยาวะ ภิกขู ภุญชันตีติ, ปะฏิเทเสตัพพัง เตหิ ภิกขูหิ “คารัย๎หัง อาวุโส ธัมมัง อาปัชชิมหา อะสัปปายัง ปาฏิเทสะนียัง, ตัง ปะฏิเทเสมาติ.</t>
+    <t>ภิกขู ปะเนวะ กุเลสุ นิมันติตา ภุญชันติ, ตัต๎ระ เจ ภิกขุนี โวสาสะมานะรูปา ฐิตา โหติ “อิธะ สูปัง เทถะ, อิธะ โอทะนัง เทถาติ, เตหิ ภิกขูหิ สา ภิกขุนี อะปะสาเทตัพพา “อะปะสักกะ ตาวะ ภะคินิ, ยาวะ ภิกขู ภุญชันตีติ, เอกัสสะปิ เจ ภิกขุโน นัปปะฏิภาเสยยะ ตัง ภิกขุนิง อะปะสาเทตุง “อะปะสักกะ ตาวะ ภะคินิ, ยาวะ ภิกขู ภุญชันตีติ, ปะฏิเทเสตัพพัง เตหิ ภิกขูหิ “คารัย๎หัง อาวุโส ธัมมัง อาปัชชิม๎หา อะสัปปายัง ปาฏิเทสะนียัง, ตัง ปะฏิเทเสมาติ.</t>
   </si>
   <si>
     <t>Bhikkhū pan’eva kulesu nimantitā bhuñjanti. Tatra ce bhikkhunī vosāsamānarūpā ṭhitā hoti: “Idha sūpaṁ detha, idha odanaṁ dethā”ti. Tehi bhikkhūhi sā bhikkhunī apasādetabbā, “Apasakka tāva bhagini, yāva bhikkhū bhuñjantī”ti: ekassa’pi ce bhikkhuno nappaṭibhāseyya taṁ bhikkhuniṁ apasādetuṁ, “apasakka tāva bhagini, yāva bhikkhū bhunjantī”ti. Paṭidesetabbaṁ tehi bhikkhūhi, “Gārayhaṁ āvuso dhammaṁ āpajjimhā asappāyaṁ pāṭidesanīyaṁ, taṁ paṭidesemā”ti.</t>
@@ -3755,7 +3755,7 @@
     <t xml:space="preserve">๓. อนึ่ง ภิกษุใดไม่ได้รับนิมนต์ก่อนมิใช่ผู้อาพาธรับของเคี้ยวก็ดีของฉันก็ดีในสกุลที่สงฆ์สมมติว่าเป็นเสขะด้วยมือของตนแล้วเคี้ยวก็ดีฉันก็ดี  อันภิกษุนั้นพึงแสดงคืนว่า"แน่ะเธอ ฉันต้องธรรมที่น่าติไม่เป็นสบาย ควรจะแสดงคืน ฉันแสดงคืนธรรมนั้น." </t>
   </si>
   <si>
-    <t>ยานิ โข ปน ตานิ อารญฺญกานิ เสนาสนานิ สาสงฺกสมฺมตานิ สปฺปฏิภยานิ, โย ปน ภิกฺขุ ตถารูเปสุ เสนาสเนสุ วิหรนฺโต1 ปุพฺเพ อปฺปฏิสํวิทิตํ ขาทนียํ วา โภชนียํ วา อชฺฌาราเม สหตฺถา ปฏิคฺคเหตฺวา อคิลาโน ขาเทยฺย วา ภุญฺเชยฺย วา, ปฏิเทเสตพฺพํ เตน ภิกฺขุนา “คารยฺหํ อาวุโส ธมฺมํ อาปชฺชึ อสปฺปายํ ปาฏิเทสนียํ, ตํ ปฏิเทเสมีติ.</t>
+    <t>ยานิ โข ปน ตานิ อารญฺญกานิ เสนาสนานิ สาสงฺกสมฺมตานิ สปฺปฏิภยานิ, โย ปน ภิกฺขุ ตถารูเปสุ เสนาสเนสุ วิหรนฺโต ปุพฺเพ อปฺปฏิสํวิทิตํ ขาทนียํ วา โภชนียํ วา อชฺฌาราเม สหตฺถา ปฏิคฺคเหตฺวา อคิลาโน ขาเทยฺย วา ภุญฺเชยฺย วา, ปฏิเทเสตพฺพํ เตน ภิกฺขุนา “คารยฺหํ อาวุโส ธมฺมํ อาปชฺชึ อสปฺปายํ ปาฏิเทสนียํ, ตํ ปฏิเทเสมีติ.</t>
   </si>
   <si>
     <t>ยานิ โข ปะนะ ตานิ อารัญญะกานิ เสนาสะนานิ สาสังกะสัมมะตานิ สัปปะฏิภะยานิ, โย ปะนะ ภิกขุ ตะถารูเปสุ เสนาสะเนสุ วิหะรันโต ปุพเพ อัปปะฏิสังวิทิตัง ขาทะนียัง วา โภชะนียัง วา อัชฌาราเม สะหัตถา ปะฏิคคะเหต๎วา อะคิลาโน ขาเทยยะ วา ภุญเชยยะ วา, ปะฏิเทเสตัพพัง เตนะ ภิกขุนา “คารัย๎หัง อาวุโส ธัมมัง อาปัชชิง อะสัปปายัง ปาฏิเทสะนียัง, ตัง ปะฏิเทเสมีติ.</t>
@@ -3896,7 +3896,7 @@
         <rFont val="Arial"/>
         <color theme="1"/>
       </rPr>
-      <t>อิเม โข ปะนายัส๎มันโต (ปัญจะสัตตะติ) เสขิยา ธัมมา อุทเทสัง อาคัจฉันติ.</t>
+      <t>อิเม โข ปะนายัส๎มันโต เสขิยา ธัมมา อุทเทสัง อาคัจฉันติ.</t>
     </r>
   </si>
   <si>
@@ -4032,7 +4032,7 @@
     <t>8. พึงทําศึกษาว่า "เราจักมีตาทอดลง นั่งในละแวกบ้าน."</t>
   </si>
   <si>
-    <t>“น อุกฺขิตฺตกาย อนตฺรฆเร คมิสฺสามีติ สิกฺขา กรณียา.</t>
+    <t>“น อุกฺขิตฺตกาย อนฺตรฆเร คมิสฺสามีติ สิกฺขา กรณียา.</t>
   </si>
   <si>
     <t>“นะ อุกขิตตะกายะ อันตะระฆะเร คะมิสสามีติ สิกขา กะระณียา.</t>
@@ -4044,7 +4044,7 @@
     <t>9. พึงทําศึกษาว่า "เราจักไม่ไปใน ละแวกบ้าน ด้วยทั้งเวิกผ้า."</t>
   </si>
   <si>
-    <t>“น อุกฺขิตฺตกาย อนตฺรฆเร นิสีทิสฺสามีติ สิกฺขา กรณียา.</t>
+    <t>“น อุกฺขิตฺตกาย อนฺตรฆเร นิสีทิสฺสามีติ สิกฺขา กรณียา.</t>
   </si>
   <si>
     <t>“นะ อุกขิตตะกายะ อันตะระฆะเร นิสีทิสสามีติ สิกขา กะระณียา.</t>
@@ -4320,7 +4320,7 @@
     <t>1. พึงทําศึกษาว่า "เราจักรับบิณฑบาตโดยเอื้อเฟื้อ</t>
   </si>
   <si>
-    <t>“ปตตฺสญฺญี ปิณฺฑปาตํ ปฏิคฺคเหสฺสามีติ สิกฺขา กรณียา.</t>
+    <t>“ปตฺตสญฺญี ปิณฺฑปาตํ ปฏิคฺคเหสฺสามีติ สิกฺขา กรณียา.</t>
   </si>
   <si>
     <t>“ปัตตะสัญญี ปิณฑะปาตัง ปะฏิคคะเหสสามีติ สิกขา กะระณียา.</t>
@@ -4395,7 +4395,7 @@
     <t>“สมสูปกํ ปิณฺฑปาตํ ภุญฺชิสฺสามีติ สิกฺขา กรณียา.</t>
   </si>
   <si>
-    <t>พระภิกขุปาฏิโมกข์ “สะมะสูปะกัง ปิณฑะปาตัง ภุญชิสสามีติ สิกขา กะระณียา.</t>
+    <t>“สะมะสูปะกัง ปิณฑะปาตัง ภุญชิสสามีติ สิกขา กะระณียา.</t>
   </si>
   <si>
     <t>Samasūpakaṁ piṇḍapātaṁ bhuñjissāmī’ti, sikkhā karaṇīyā.</t>
@@ -4479,7 +4479,7 @@
     <t>“น อนาหเฏ กวเฬ มุขทฺวารํ วิวริสฺสามีติ สิกฺขา กรณียา.</t>
   </si>
   <si>
-    <t>“นะ อะนาหะเฏ กะวะเฬ มุขะท๎วารัง วิวะริสสามีติ สิกขา กะระณียา.</t>
+    <t>“นะ อะนาหะเฏ กะวะเฬ มุขัท๎วารัง วิวะริสสามีติ สิกขา กะระณียา.</t>
   </si>
   <si>
     <t>Na anāhate kavaḷe mukhadvāraṁ vivarissāmī’ti, sikkhā karaṇīyā.</t>
@@ -5103,7 +5103,7 @@
         <rFont val="Arial"/>
         <color theme="1"/>
       </rPr>
-      <t xml:space="preserve">อุททิฏฐา โข อายัส๎มันโต (ปัญจะสัตตะติ) เสขิยา ธัมมา.
+      <t xml:space="preserve">อุททิฏฐา โข อายัส๎มันโต เสขิยา ธัมมา.
 ตัตถายัส๎มันเต ปุจฉามิ. กัจจิตถะ ปะริสุทธา ?
 ทุติยัมปิ ปุจฉามิ. กัจจิตถะ ปะริสุทธา ?
 ตะติยัมปิ ปุจฉามิ. กัจจิตถะ ปะริสุทธา ?
@@ -5187,7 +5187,7 @@
       </rPr>
       <t xml:space="preserve">
 อิเม โข ปนายสฺมนฺโต สตฺตาธิกรณสมถา ธมฺมา อุทฺเทสํ อาคจฺฉนฺติ.
-อุปฺปนฺนุปฺปนฺนานํ อธิกรณานํ สมถาย วูปสมาย สมฺมุขาวินโย ทาตพฺโพ, สติวินโย ทาตพโฺพ, อมูฬฺหวินโย ทาตพฺโพ, ปฏิญฺญาตกรณํ, เยภุยฺยสิกา, ตสฺส ปาปิยสิกา , ติณวตฺถารโกติ.
+อุปฺปนฺนุปฺปนฺนานํ อธิกรณานํ สมถาย วูปสมาย สมฺมุขาวินโย ทาตพฺโพ, สติวินโย ทาตพฺโพ, อมูฬฺหวินโย ทาตพฺโพ, ปฏิญฺญาตกรณํ, เยภุยฺยสิกา, ตสฺส ปาปิยสิกา , ติณวตฺถารโกติ.
 อุทฺทิฏฺฐา โข อายสฺมนฺโต สตฺตาธิกรณสมถา ธมฺมา.
 ตตฺถายสฺมนฺเต ปุจฺฉามิ: กจฺจิตฺถ ปริสุทฺธา ?
 ทุติยมฺปิ ปุจฺฉามิ: กจฺจิตฺถ ปริสุทฺธา ?
@@ -5358,7 +5358,7 @@
 อุททิฏฐา ติงสะ นิสสัคคิยา ปาจิตติยา ธัมมา,
 อุททิฏฐา เท๎วนะวุติ ปาจิตติยา ธัมมา,
 อุททิฏฐา จัตตาโร ปาฏิเทสะนียา ธัมมา,
-อุททิฏฐา (ปัญจะสัตตะติ) เสขิยา ธัมมา,
+อุททิฏฐา เสขิยา ธัมมา,
 อุททิฏฐา สัตตาธิกะระณะสะมะถา ธัมมา,
 เอตตะกันตัสสะ ภะคะวะโต สุตตาคะตัง สุตตะปะริยาปันนัง อัน๎วัฑฒะมาสัง อุทเทสัง อาคัจฉะติ. ตัตถะ สัพเพเหวะ สะมัคเคหิ สัมโมทะมาเนหิ อะวิวะทะมาเนหิ สิกขิตัพพันติ.
 </t>
@@ -5449,12 +5449,12 @@
         <color theme="1"/>
       </rPr>
       <t xml:space="preserve">
-นตฺถิ เม สรณํ อญฺญํ พุทโธ เม สรณํ วรํ
-เอเตน สจฺจวชฺเชน โสตฺถิ เม โหตุ สพฺพทา
+นตฺถิ เม สรณํ อญฺญํ พุทฺโธ เม สรณํ วรํ
+เอเตน สจฺจวชฺเชน โสตฺถิ เต โหตุ สพฺพทา
 นตฺถิ เม สรณํ อญฺญํ ธมฺโม เม สรณํ วรํ
-เอเตน สจฺจวชฺเชน โสตฺถิ เม โหตุ สพฺพทา
+เอเตน สจฺจวชฺเชน โสตฺถิ เต โหตุ สพฺพทา
 นตฺถิ เม สรณํ อญฺญํ สงฺโฆ เม สรณํ วรํ
-เอเตน สจฺจวชฺเชน โสตฺถิ เม โหตุ สพฺพทา
+เอเตน สจฺจวชฺเชน โสตฺถิ เต โหตุ สพฺพทา
 </t>
     </r>
   </si>
@@ -5473,11 +5473,11 @@
         <rFont val="Arial"/>
         <color theme="1"/>
       </rPr>
-      <t>นัตถิ เม สะระนัง อัญญัง พุทโธ เม สะระณัง วะรัง,
+      <t>นัตถิ เม สะระณัง อัญญัง พุทโธ เม สะระณัง วะรัง,
 เอเตนะ สัจจะวัชเชนะ โสตถิ เต โหตุ สัพพะทา ฯ
-นัตถิ เม สะระนัง อัญญัง ธัมโม เม สะระณัง วะรัง,
+นัตถิ เม สะระณัง อัญญัง ธัมโม เม สะระณัง วะรัง,
 เอเตนะ สัจจะวัชเชนะ โสตถิ เต โหตุ สัพพะทา ฯ
-นัตถิ เม สะระนัง อัญญัง สังโฆ เม สะระณัง วะรัง,
+นัตถิ เม สะระณัง อัญญัง สังโฆ เม สะระณัง วะรัง,
 เอเตนะ สัจจะวัชเชนะ โสตถิ เต โหตุ สัพพะทา ฯ</t>
     </r>
   </si>
@@ -5681,7 +5681,7 @@
       <t xml:space="preserve">
 ฉินทะ โสตัง ปะรักกัมมะ กาเม ปะนูทะ พ๎ราห๎มะณะ,
 นัปปะหายะ มุนิ กาเม เนกัตตะมุปะปัชชะติ,
-กะยิรา เจ กะยิราเถนัง ทัฬหะเมนัง ปะรักกะเม,
+กะยิรา เจ กะยิราเถนัง ทัฬ๎หะเมนัง ปะรักกะเม,
 สิถิโล หิ ปะริพพาโช ภิยโย อากิระเต ระชัง,
 อะกะตัง ทุกกะฏัง เสยโย ปัจฉา ตัปปะติ ทุกกะฏัง,
 กะตัญจะ สุกะตัง เสยโย ยัง กัต๎วา นานุตัปปะติ,
@@ -5740,7 +5740,7 @@
 ท่านจงพยายามตัดตัณหาเพียงดังกระแสนํ้าเสีย, จงถ่ายถอนกามทั้งหลายเสียเถิดนะพราหมณ์ ;
 นัปปะหายะ มุนิ กาเม, เนกัตตะมุปะปัชชะติ,
 เพราะมุนีไม่ละกามทั้งหลายแล้ว,จะเข้าถึงความเป็นคนผู้เดียวไม่ได้ ;
-กะยิรา เจ กะยิราเถนัง, ทัฬหะเมนัง ปะรักกะเม,
+กะยิรา เจ กะยิราเถนัง, ทัฬ๎หะเมนัง ปะรักกะเม,
 ถ้าจะทำ ก็พึงทำกิจนั้นเถิด แต่พึงบากบั่นทำกิจนั้น ให้จริง ;
 สิถิโล หิ ปะริพพาโช, ภิยโย อากิระเต ระชัง,
 เพราะสมณธรรมเครื่องละเว้นที่ย่อหย่อน, ยิ่งโปรยโทษดุจธุลีลง ;
@@ -14018,7 +14018,7 @@
       </c>
       <c r="H43" s="2"/>
     </row>
-    <row r="44" hidden="1" outlineLevel="1">
+    <row r="44" outlineLevel="1">
       <c r="A44" s="1" t="s">
         <v>140</v>
       </c>
@@ -14042,7 +14042,7 @@
       </c>
       <c r="H44" s="2"/>
     </row>
-    <row r="45" hidden="1" outlineLevel="1">
+    <row r="45" outlineLevel="1">
       <c r="A45" s="1" t="s">
         <v>140</v>
       </c>
@@ -14066,7 +14066,7 @@
       </c>
       <c r="H45" s="2"/>
     </row>
-    <row r="46" hidden="1" outlineLevel="1">
+    <row r="46" outlineLevel="1">
       <c r="A46" s="1" t="s">
         <v>140</v>
       </c>
@@ -14090,7 +14090,7 @@
       </c>
       <c r="H46" s="2"/>
     </row>
-    <row r="47" hidden="1" outlineLevel="1">
+    <row r="47" outlineLevel="1">
       <c r="A47" s="1" t="s">
         <v>140</v>
       </c>
@@ -14114,7 +14114,7 @@
       </c>
       <c r="H47" s="2"/>
     </row>
-    <row r="48" hidden="1" outlineLevel="1">
+    <row r="48" outlineLevel="1">
       <c r="A48" s="1" t="s">
         <v>140</v>
       </c>
@@ -14138,7 +14138,7 @@
       </c>
       <c r="H48" s="2"/>
     </row>
-    <row r="49" hidden="1" outlineLevel="1">
+    <row r="49" outlineLevel="1">
       <c r="A49" s="1" t="s">
         <v>140</v>
       </c>
@@ -14162,7 +14162,7 @@
       </c>
       <c r="H49" s="2"/>
     </row>
-    <row r="50" hidden="1" outlineLevel="1">
+    <row r="50" outlineLevel="1">
       <c r="A50" s="1" t="s">
         <v>140</v>
       </c>
@@ -14186,7 +14186,7 @@
       </c>
       <c r="H50" s="2"/>
     </row>
-    <row r="51" hidden="1" outlineLevel="1">
+    <row r="51" outlineLevel="1">
       <c r="A51" s="1" t="s">
         <v>140</v>
       </c>
@@ -14210,7 +14210,7 @@
       </c>
       <c r="H51" s="2"/>
     </row>
-    <row r="52" hidden="1" outlineLevel="1">
+    <row r="52" outlineLevel="1">
       <c r="A52" s="1" t="s">
         <v>140</v>
       </c>
@@ -14234,7 +14234,7 @@
       </c>
       <c r="H52" s="2"/>
     </row>
-    <row r="53" collapsed="1">
+    <row r="53">
       <c r="A53" s="1" t="s">
         <v>140</v>
       </c>
@@ -14258,7 +14258,7 @@
       </c>
       <c r="H53" s="2"/>
     </row>
-    <row r="54" hidden="1" outlineLevel="1">
+    <row r="54" outlineLevel="1">
       <c r="A54" s="1" t="s">
         <v>140</v>
       </c>
@@ -14282,7 +14282,7 @@
       </c>
       <c r="H54" s="2"/>
     </row>
-    <row r="55" hidden="1" outlineLevel="1">
+    <row r="55" outlineLevel="1">
       <c r="A55" s="1" t="s">
         <v>140</v>
       </c>
@@ -14306,7 +14306,7 @@
       </c>
       <c r="H55" s="2"/>
     </row>
-    <row r="56" hidden="1" outlineLevel="1">
+    <row r="56" outlineLevel="1">
       <c r="A56" s="1" t="s">
         <v>140</v>
       </c>
@@ -14330,7 +14330,7 @@
       </c>
       <c r="H56" s="2"/>
     </row>
-    <row r="57" hidden="1" outlineLevel="1">
+    <row r="57" outlineLevel="1">
       <c r="A57" s="1" t="s">
         <v>140</v>
       </c>
@@ -14354,7 +14354,7 @@
       </c>
       <c r="H57" s="2"/>
     </row>
-    <row r="58" hidden="1" outlineLevel="1">
+    <row r="58" outlineLevel="1">
       <c r="A58" s="1" t="s">
         <v>140</v>
       </c>
@@ -14378,7 +14378,7 @@
       </c>
       <c r="H58" s="2"/>
     </row>
-    <row r="59" hidden="1" outlineLevel="1">
+    <row r="59" outlineLevel="1">
       <c r="A59" s="1" t="s">
         <v>140</v>
       </c>
@@ -14402,7 +14402,7 @@
       </c>
       <c r="H59" s="2"/>
     </row>
-    <row r="60" hidden="1" outlineLevel="1">
+    <row r="60" outlineLevel="1">
       <c r="A60" s="1" t="s">
         <v>140</v>
       </c>
@@ -14426,7 +14426,7 @@
       </c>
       <c r="H60" s="2"/>
     </row>
-    <row r="61" hidden="1" outlineLevel="1">
+    <row r="61" outlineLevel="1">
       <c r="A61" s="1" t="s">
         <v>140</v>
       </c>
@@ -14450,7 +14450,7 @@
       </c>
       <c r="H61" s="2"/>
     </row>
-    <row r="62" hidden="1" outlineLevel="1">
+    <row r="62" outlineLevel="1">
       <c r="A62" s="1" t="s">
         <v>140</v>
       </c>
@@ -14474,7 +14474,7 @@
       </c>
       <c r="H62" s="2"/>
     </row>
-    <row r="63" collapsed="1">
+    <row r="63">
       <c r="A63" s="1" t="s">
         <v>140</v>
       </c>
@@ -15506,7 +15506,7 @@
       </c>
       <c r="H105" s="2"/>
     </row>
-    <row r="106" hidden="1" outlineLevel="2">
+    <row r="106" outlineLevel="2">
       <c r="A106" s="1" t="s">
         <v>269</v>
       </c>
@@ -15530,7 +15530,7 @@
       </c>
       <c r="H106" s="2"/>
     </row>
-    <row r="107" hidden="1" outlineLevel="2">
+    <row r="107" outlineLevel="2">
       <c r="A107" s="1" t="s">
         <v>269</v>
       </c>
@@ -15554,7 +15554,7 @@
       </c>
       <c r="H107" s="2"/>
     </row>
-    <row r="108" hidden="1" outlineLevel="2">
+    <row r="108" outlineLevel="2">
       <c r="A108" s="1" t="s">
         <v>269</v>
       </c>
@@ -15578,7 +15578,7 @@
       </c>
       <c r="H108" s="2"/>
     </row>
-    <row r="109" hidden="1" outlineLevel="2">
+    <row r="109" outlineLevel="2">
       <c r="A109" s="1" t="s">
         <v>269</v>
       </c>
@@ -15602,7 +15602,7 @@
       </c>
       <c r="H109" s="2"/>
     </row>
-    <row r="110" hidden="1" outlineLevel="2">
+    <row r="110" outlineLevel="2">
       <c r="A110" s="1" t="s">
         <v>269</v>
       </c>
@@ -15626,7 +15626,7 @@
       </c>
       <c r="H110" s="2"/>
     </row>
-    <row r="111" hidden="1" outlineLevel="2">
+    <row r="111" outlineLevel="2">
       <c r="A111" s="1" t="s">
         <v>269</v>
       </c>
@@ -15650,7 +15650,7 @@
       </c>
       <c r="H111" s="2"/>
     </row>
-    <row r="112" hidden="1" outlineLevel="2">
+    <row r="112" outlineLevel="2">
       <c r="A112" s="1" t="s">
         <v>269</v>
       </c>
@@ -15674,7 +15674,7 @@
       </c>
       <c r="H112" s="2"/>
     </row>
-    <row r="113" hidden="1" outlineLevel="2">
+    <row r="113" outlineLevel="2">
       <c r="A113" s="1" t="s">
         <v>269</v>
       </c>
@@ -15698,7 +15698,7 @@
       </c>
       <c r="H113" s="2"/>
     </row>
-    <row r="114" hidden="1" outlineLevel="2">
+    <row r="114" outlineLevel="2">
       <c r="A114" s="1" t="s">
         <v>269</v>
       </c>
@@ -15722,7 +15722,7 @@
       </c>
       <c r="H114" s="2"/>
     </row>
-    <row r="115" outlineLevel="1" collapsed="1">
+    <row r="115" outlineLevel="1">
       <c r="A115" s="1" t="s">
         <v>269</v>
       </c>
@@ -15746,7 +15746,7 @@
       </c>
       <c r="H115" s="2"/>
     </row>
-    <row r="116" hidden="1" outlineLevel="2">
+    <row r="116" outlineLevel="2">
       <c r="A116" s="1" t="s">
         <v>269</v>
       </c>
@@ -15770,7 +15770,7 @@
       </c>
       <c r="H116" s="2"/>
     </row>
-    <row r="117" hidden="1" outlineLevel="2">
+    <row r="117" outlineLevel="2">
       <c r="A117" s="1" t="s">
         <v>269</v>
       </c>
@@ -15794,7 +15794,7 @@
       </c>
       <c r="H117" s="2"/>
     </row>
-    <row r="118" hidden="1" outlineLevel="2">
+    <row r="118" outlineLevel="2">
       <c r="A118" s="1" t="s">
         <v>269</v>
       </c>
@@ -15818,7 +15818,7 @@
       </c>
       <c r="H118" s="2"/>
     </row>
-    <row r="119" hidden="1" outlineLevel="2">
+    <row r="119" outlineLevel="2">
       <c r="A119" s="1" t="s">
         <v>269</v>
       </c>
@@ -15842,7 +15842,7 @@
       </c>
       <c r="H119" s="2"/>
     </row>
-    <row r="120" hidden="1" outlineLevel="2">
+    <row r="120" outlineLevel="2">
       <c r="A120" s="1" t="s">
         <v>269</v>
       </c>
@@ -15866,7 +15866,7 @@
       </c>
       <c r="H120" s="2"/>
     </row>
-    <row r="121" hidden="1" outlineLevel="2">
+    <row r="121" outlineLevel="2">
       <c r="A121" s="1" t="s">
         <v>269</v>
       </c>
@@ -15890,7 +15890,7 @@
       </c>
       <c r="H121" s="2"/>
     </row>
-    <row r="122" hidden="1" outlineLevel="2">
+    <row r="122" outlineLevel="2">
       <c r="A122" s="1" t="s">
         <v>269</v>
       </c>
@@ -15914,7 +15914,7 @@
       </c>
       <c r="H122" s="2"/>
     </row>
-    <row r="123" hidden="1" outlineLevel="2">
+    <row r="123" outlineLevel="2">
       <c r="A123" s="1" t="s">
         <v>269</v>
       </c>
@@ -15938,7 +15938,7 @@
       </c>
       <c r="H123" s="2"/>
     </row>
-    <row r="124" hidden="1" outlineLevel="2">
+    <row r="124" outlineLevel="2">
       <c r="A124" s="1" t="s">
         <v>269</v>
       </c>
@@ -15962,7 +15962,7 @@
       </c>
       <c r="H124" s="2"/>
     </row>
-    <row r="125" outlineLevel="1" collapsed="1">
+    <row r="125" outlineLevel="1">
       <c r="A125" s="1" t="s">
         <v>269</v>
       </c>
@@ -15986,7 +15986,7 @@
       </c>
       <c r="H125" s="2"/>
     </row>
-    <row r="126" hidden="1" outlineLevel="2">
+    <row r="126" outlineLevel="2">
       <c r="A126" s="1" t="s">
         <v>269</v>
       </c>
@@ -16010,7 +16010,7 @@
       </c>
       <c r="H126" s="2"/>
     </row>
-    <row r="127" hidden="1" outlineLevel="2">
+    <row r="127" outlineLevel="2">
       <c r="A127" s="1" t="s">
         <v>269</v>
       </c>
@@ -16034,7 +16034,7 @@
       </c>
       <c r="H127" s="2"/>
     </row>
-    <row r="128" hidden="1" outlineLevel="2">
+    <row r="128" outlineLevel="2">
       <c r="A128" s="1" t="s">
         <v>269</v>
       </c>
@@ -16058,7 +16058,7 @@
       </c>
       <c r="H128" s="2"/>
     </row>
-    <row r="129" hidden="1" outlineLevel="2">
+    <row r="129" outlineLevel="2">
       <c r="A129" s="1" t="s">
         <v>269</v>
       </c>
@@ -16082,7 +16082,7 @@
       </c>
       <c r="H129" s="2"/>
     </row>
-    <row r="130" hidden="1" outlineLevel="2">
+    <row r="130" outlineLevel="2">
       <c r="A130" s="1" t="s">
         <v>269</v>
       </c>
@@ -16106,7 +16106,7 @@
       </c>
       <c r="H130" s="2"/>
     </row>
-    <row r="131" hidden="1" outlineLevel="2">
+    <row r="131" outlineLevel="2">
       <c r="A131" s="1" t="s">
         <v>269</v>
       </c>
@@ -16130,7 +16130,7 @@
       </c>
       <c r="H131" s="2"/>
     </row>
-    <row r="132" hidden="1" outlineLevel="2">
+    <row r="132" outlineLevel="2">
       <c r="A132" s="1" t="s">
         <v>269</v>
       </c>
@@ -16154,7 +16154,7 @@
       </c>
       <c r="H132" s="2"/>
     </row>
-    <row r="133" hidden="1" outlineLevel="2">
+    <row r="133" outlineLevel="2">
       <c r="A133" s="1" t="s">
         <v>269</v>
       </c>
@@ -16178,7 +16178,7 @@
       </c>
       <c r="H133" s="2"/>
     </row>
-    <row r="134" hidden="1" outlineLevel="2">
+    <row r="134" outlineLevel="2">
       <c r="A134" s="1" t="s">
         <v>269</v>
       </c>
@@ -16202,7 +16202,7 @@
       </c>
       <c r="H134" s="2"/>
     </row>
-    <row r="135" outlineLevel="1" collapsed="1">
+    <row r="135" outlineLevel="1">
       <c r="A135" s="1" t="s">
         <v>269</v>
       </c>
@@ -16226,7 +16226,7 @@
       </c>
       <c r="H135" s="2"/>
     </row>
-    <row r="136" hidden="1" outlineLevel="2">
+    <row r="136" outlineLevel="2">
       <c r="A136" s="1" t="s">
         <v>269</v>
       </c>
@@ -16250,7 +16250,7 @@
       </c>
       <c r="H136" s="2"/>
     </row>
-    <row r="137" hidden="1" outlineLevel="2">
+    <row r="137" outlineLevel="2">
       <c r="A137" s="1" t="s">
         <v>269</v>
       </c>
@@ -16274,7 +16274,7 @@
       </c>
       <c r="H137" s="2"/>
     </row>
-    <row r="138" hidden="1" outlineLevel="2">
+    <row r="138" outlineLevel="2">
       <c r="A138" s="1" t="s">
         <v>269</v>
       </c>
@@ -16298,7 +16298,7 @@
       </c>
       <c r="H138" s="2"/>
     </row>
-    <row r="139" hidden="1" outlineLevel="2">
+    <row r="139" outlineLevel="2">
       <c r="A139" s="1" t="s">
         <v>269</v>
       </c>
@@ -16322,7 +16322,7 @@
       </c>
       <c r="H139" s="2"/>
     </row>
-    <row r="140" hidden="1" outlineLevel="2">
+    <row r="140" outlineLevel="2">
       <c r="A140" s="1" t="s">
         <v>269</v>
       </c>
@@ -16346,7 +16346,7 @@
       </c>
       <c r="H140" s="2"/>
     </row>
-    <row r="141" hidden="1" outlineLevel="2">
+    <row r="141" outlineLevel="2">
       <c r="A141" s="1" t="s">
         <v>269</v>
       </c>
@@ -16370,7 +16370,7 @@
       </c>
       <c r="H141" s="2"/>
     </row>
-    <row r="142" hidden="1" outlineLevel="2">
+    <row r="142" outlineLevel="2">
       <c r="A142" s="1" t="s">
         <v>269</v>
       </c>
@@ -16394,7 +16394,7 @@
       </c>
       <c r="H142" s="2"/>
     </row>
-    <row r="143" hidden="1" outlineLevel="2">
+    <row r="143" outlineLevel="2">
       <c r="A143" s="1" t="s">
         <v>269</v>
       </c>
@@ -16418,7 +16418,7 @@
       </c>
       <c r="H143" s="2"/>
     </row>
-    <row r="144" hidden="1" outlineLevel="2">
+    <row r="144" outlineLevel="2">
       <c r="A144" s="1" t="s">
         <v>269</v>
       </c>
@@ -16442,7 +16442,7 @@
       </c>
       <c r="H144" s="2"/>
     </row>
-    <row r="145" hidden="1" outlineLevel="2">
+    <row r="145" outlineLevel="2">
       <c r="A145" s="1" t="s">
         <v>269</v>
       </c>
@@ -16466,7 +16466,7 @@
       </c>
       <c r="H145" s="2"/>
     </row>
-    <row r="146" hidden="1" outlineLevel="2">
+    <row r="146" outlineLevel="2">
       <c r="A146" s="1" t="s">
         <v>269</v>
       </c>
@@ -16490,7 +16490,7 @@
       </c>
       <c r="H146" s="2"/>
     </row>
-    <row r="147" outlineLevel="1" collapsed="1">
+    <row r="147" outlineLevel="1">
       <c r="A147" s="1" t="s">
         <v>269</v>
       </c>
@@ -16514,7 +16514,7 @@
       </c>
       <c r="H147" s="2"/>
     </row>
-    <row r="148" hidden="1" outlineLevel="2">
+    <row r="148" outlineLevel="2">
       <c r="A148" s="1" t="s">
         <v>269</v>
       </c>
@@ -16538,7 +16538,7 @@
       </c>
       <c r="H148" s="2"/>
     </row>
-    <row r="149" hidden="1" outlineLevel="2">
+    <row r="149" outlineLevel="2">
       <c r="A149" s="1" t="s">
         <v>269</v>
       </c>
@@ -16562,7 +16562,7 @@
       </c>
       <c r="H149" s="2"/>
     </row>
-    <row r="150" hidden="1" outlineLevel="2">
+    <row r="150" outlineLevel="2">
       <c r="A150" s="1" t="s">
         <v>269</v>
       </c>
@@ -16586,7 +16586,7 @@
       </c>
       <c r="H150" s="2"/>
     </row>
-    <row r="151" hidden="1" outlineLevel="2">
+    <row r="151" outlineLevel="2">
       <c r="A151" s="1" t="s">
         <v>269</v>
       </c>
@@ -16610,7 +16610,7 @@
       </c>
       <c r="H151" s="2"/>
     </row>
-    <row r="152" hidden="1" outlineLevel="2">
+    <row r="152" outlineLevel="2">
       <c r="A152" s="1" t="s">
         <v>269</v>
       </c>
@@ -16634,7 +16634,7 @@
       </c>
       <c r="H152" s="2"/>
     </row>
-    <row r="153" hidden="1" outlineLevel="2">
+    <row r="153" outlineLevel="2">
       <c r="A153" s="1" t="s">
         <v>269</v>
       </c>
@@ -16658,7 +16658,7 @@
       </c>
       <c r="H153" s="2"/>
     </row>
-    <row r="154" hidden="1" outlineLevel="2">
+    <row r="154" outlineLevel="2">
       <c r="A154" s="1" t="s">
         <v>269</v>
       </c>
@@ -16682,7 +16682,7 @@
       </c>
       <c r="H154" s="2"/>
     </row>
-    <row r="155" hidden="1" outlineLevel="2">
+    <row r="155" outlineLevel="2">
       <c r="A155" s="1" t="s">
         <v>269</v>
       </c>
@@ -16706,7 +16706,7 @@
       </c>
       <c r="H155" s="2"/>
     </row>
-    <row r="156" hidden="1" outlineLevel="2">
+    <row r="156" outlineLevel="2">
       <c r="A156" s="1" t="s">
         <v>269</v>
       </c>
@@ -16730,7 +16730,7 @@
       </c>
       <c r="H156" s="2"/>
     </row>
-    <row r="157" outlineLevel="1" collapsed="1">
+    <row r="157" outlineLevel="1">
       <c r="A157" s="1" t="s">
         <v>269</v>
       </c>

</xml_diff>